<commit_message>
edited gantt chart in schedule
</commit_message>
<xml_diff>
--- a/schedule/G6T6 SPM Gantt Chart.xlsx
+++ b/schedule/G6T6 SPM Gantt Chart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zychoo.2018\Google Drive\SMU\Y2S1\SPM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\project-g6t6\schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1FE3C0-0D96-4960-B2EE-8888C0D79DC9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C78342E-A09D-4948-95FE-9A09B41DF551}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="132">
   <si>
     <t>TASK NAME</t>
   </si>
@@ -340,6 +340,7 @@
         <i/>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>File</t>
     </r>
@@ -348,6 +349,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">, the select </t>
     </r>
@@ -356,6 +358,7 @@
         <i/>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Make a Copy</t>
     </r>
@@ -364,6 +367,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>.</t>
     </r>
@@ -456,7 +460,10 @@
     <t>2.4 Begin preparing power point slides for week 7</t>
   </si>
   <si>
-    <t>Doesn't include validation</t>
+    <t>Doesn't include validation Incomplete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      3.2.4 admin-bootstrap function (continued)</t>
   </si>
 </sst>
 </file>
@@ -468,7 +475,7 @@
     <numFmt numFmtId="165" formatCode="m&quot;/&quot;d"/>
     <numFmt numFmtId="166" formatCode="m/d"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -479,50 +486,60 @@
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF666666"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF434343"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF62676D"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="26"/>
       <color rgb="FF576C88"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -539,6 +556,7 @@
       <sz val="10"/>
       <color rgb="FF576C88"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -546,26 +564,37 @@
       <sz val="14"/>
       <color rgb="FF57BB8A"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF576C88"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="16">
@@ -794,7 +823,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -979,46 +1008,57 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1531,7 +1571,7 @@
                     <a:latin typeface="Roboto"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr/>
+                <a:endParaRPr lang="en-SG"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1604,6 +1644,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
+                  <a:rPr lang="en-SG"/>
                   <a:t>Days of the Month</a:t>
                 </a:r>
               </a:p>
@@ -1998,7 +2039,7 @@
                     <a:latin typeface="Roboto"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr/>
+                <a:endParaRPr lang="en-SG"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2071,6 +2112,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
+                  <a:rPr lang="en-SG"/>
                   <a:t>Days of the Month</a:t>
                 </a:r>
               </a:p>
@@ -2491,13 +2533,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:CI1022"/>
+  <dimension ref="A1:CI1023"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="W14" sqref="W14"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2505,151 +2547,154 @@
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="41.33203125" customWidth="1"/>
     <col min="3" max="4" width="11.88671875" customWidth="1"/>
-    <col min="5" max="8" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" customWidth="1"/>
     <col min="9" max="9" width="10.33203125" customWidth="1"/>
     <col min="10" max="10" width="12.33203125" customWidth="1"/>
     <col min="11" max="87" width="4.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:87">
-      <c r="A1" s="97"/>
-      <c r="B1" s="97" t="s">
+    <row r="1" spans="1:87" ht="14.4">
+      <c r="A1" s="99"/>
+      <c r="B1" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="97" t="s">
+      <c r="C1" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="97" t="s">
+      <c r="D1" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="97" t="s">
+      <c r="E1" s="99" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="97" t="s">
+      <c r="F1" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="97" t="s">
+      <c r="G1" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="97" t="s">
+      <c r="H1" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="99" t="s">
+      <c r="I1" s="106" t="s">
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="101" t="s">
+      <c r="K1" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="95"/>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
-      <c r="O1" s="95"/>
+      <c r="L1" s="103"/>
+      <c r="M1" s="103"/>
+      <c r="N1" s="103"/>
+      <c r="O1" s="103"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
-      <c r="R1" s="96" t="s">
+      <c r="R1" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="95"/>
-      <c r="T1" s="95"/>
-      <c r="U1" s="95"/>
-      <c r="V1" s="95"/>
+      <c r="S1" s="103"/>
+      <c r="T1" s="103"/>
+      <c r="U1" s="103"/>
+      <c r="V1" s="103"/>
       <c r="W1" s="3"/>
       <c r="X1" s="3"/>
-      <c r="Y1" s="94" t="s">
+      <c r="Y1" s="105" t="s">
         <v>11</v>
       </c>
-      <c r="Z1" s="95"/>
-      <c r="AA1" s="95"/>
-      <c r="AB1" s="95"/>
-      <c r="AC1" s="95"/>
+      <c r="Z1" s="103"/>
+      <c r="AA1" s="103"/>
+      <c r="AB1" s="103"/>
+      <c r="AC1" s="103"/>
       <c r="AD1" s="2"/>
       <c r="AE1" s="2"/>
-      <c r="AF1" s="96" t="s">
+      <c r="AF1" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="AG1" s="95"/>
-      <c r="AH1" s="95"/>
-      <c r="AI1" s="95"/>
-      <c r="AJ1" s="95"/>
+      <c r="AG1" s="103"/>
+      <c r="AH1" s="103"/>
+      <c r="AI1" s="103"/>
+      <c r="AJ1" s="103"/>
       <c r="AK1" s="3"/>
       <c r="AL1" s="3"/>
-      <c r="AM1" s="94" t="s">
+      <c r="AM1" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="AN1" s="95"/>
-      <c r="AO1" s="95"/>
-      <c r="AP1" s="95"/>
-      <c r="AQ1" s="95"/>
+      <c r="AN1" s="103"/>
+      <c r="AO1" s="103"/>
+      <c r="AP1" s="103"/>
+      <c r="AQ1" s="103"/>
       <c r="AR1" s="2"/>
       <c r="AS1" s="2"/>
-      <c r="AT1" s="96" t="s">
+      <c r="AT1" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="AU1" s="95"/>
-      <c r="AV1" s="95"/>
-      <c r="AW1" s="95"/>
-      <c r="AX1" s="95"/>
+      <c r="AU1" s="103"/>
+      <c r="AV1" s="103"/>
+      <c r="AW1" s="103"/>
+      <c r="AX1" s="103"/>
       <c r="AY1" s="3"/>
       <c r="AZ1" s="3"/>
-      <c r="BA1" s="94" t="s">
+      <c r="BA1" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="BB1" s="95"/>
-      <c r="BC1" s="95"/>
-      <c r="BD1" s="95"/>
-      <c r="BE1" s="95"/>
+      <c r="BB1" s="103"/>
+      <c r="BC1" s="103"/>
+      <c r="BD1" s="103"/>
+      <c r="BE1" s="103"/>
       <c r="BF1" s="2"/>
       <c r="BG1" s="2"/>
-      <c r="BH1" s="96" t="s">
+      <c r="BH1" s="102" t="s">
         <v>16</v>
       </c>
-      <c r="BI1" s="95"/>
-      <c r="BJ1" s="95"/>
-      <c r="BK1" s="95"/>
-      <c r="BL1" s="95"/>
+      <c r="BI1" s="103"/>
+      <c r="BJ1" s="103"/>
+      <c r="BK1" s="103"/>
+      <c r="BL1" s="103"/>
       <c r="BM1" s="3"/>
       <c r="BN1" s="3"/>
-      <c r="BO1" s="94" t="s">
+      <c r="BO1" s="105" t="s">
         <v>17</v>
       </c>
-      <c r="BP1" s="95"/>
-      <c r="BQ1" s="95"/>
-      <c r="BR1" s="95"/>
-      <c r="BS1" s="95"/>
+      <c r="BP1" s="103"/>
+      <c r="BQ1" s="103"/>
+      <c r="BR1" s="103"/>
+      <c r="BS1" s="103"/>
       <c r="BT1" s="2"/>
       <c r="BU1" s="2"/>
-      <c r="BV1" s="96" t="s">
+      <c r="BV1" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="BW1" s="95"/>
-      <c r="BX1" s="95"/>
-      <c r="BY1" s="95"/>
-      <c r="BZ1" s="95"/>
+      <c r="BW1" s="103"/>
+      <c r="BX1" s="103"/>
+      <c r="BY1" s="103"/>
+      <c r="BZ1" s="103"/>
       <c r="CA1" s="3"/>
       <c r="CB1" s="3"/>
-      <c r="CC1" s="94" t="s">
+      <c r="CC1" s="105" t="s">
         <v>19</v>
       </c>
-      <c r="CD1" s="95"/>
-      <c r="CE1" s="95"/>
-      <c r="CF1" s="95"/>
-      <c r="CG1" s="95"/>
+      <c r="CD1" s="103"/>
+      <c r="CE1" s="103"/>
+      <c r="CF1" s="103"/>
+      <c r="CG1" s="103"/>
       <c r="CH1" s="2"/>
       <c r="CI1" s="2"/>
     </row>
-    <row r="2" spans="1:87">
-      <c r="A2" s="98"/>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="100"/>
+    <row r="2" spans="1:87" ht="14.4">
+      <c r="A2" s="100"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="107"/>
       <c r="J2" s="1"/>
       <c r="K2" s="4" t="s">
         <v>20</v>
@@ -2883,18 +2928,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:87">
+    <row r="3" spans="1:87" ht="15.6">
       <c r="A3" s="10" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="11"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="103"/>
-      <c r="E3" s="103"/>
-      <c r="F3" s="103"/>
-      <c r="G3" s="103"/>
-      <c r="H3" s="103"/>
-      <c r="I3" s="103"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
       <c r="J3" s="12"/>
       <c r="K3" s="13"/>
       <c r="L3" s="14"/>
@@ -2974,7 +3019,7 @@
       <c r="CH3" s="12"/>
       <c r="CI3" s="12"/>
     </row>
-    <row r="4" spans="1:87">
+    <row r="4" spans="1:87" ht="14.4">
       <c r="A4" s="16">
         <v>1</v>
       </c>
@@ -3063,7 +3108,7 @@
       <c r="CH4" s="25"/>
       <c r="CI4" s="25"/>
     </row>
-    <row r="5" spans="1:87">
+    <row r="5" spans="1:87" ht="14.4">
       <c r="A5" s="16"/>
       <c r="B5" s="17" t="s">
         <v>28</v>
@@ -3075,10 +3120,14 @@
         <v>29</v>
       </c>
       <c r="E5" s="26">
-        <v>2</v>
-      </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
+        <v>2.5</v>
+      </c>
+      <c r="F5" s="114">
+        <v>43721.645833333336</v>
+      </c>
+      <c r="G5" s="114">
+        <v>43721.770833333336</v>
+      </c>
       <c r="H5" s="19" t="s">
         <v>30</v>
       </c>
@@ -3164,7 +3213,7 @@
       <c r="CH5" s="25"/>
       <c r="CI5" s="25"/>
     </row>
-    <row r="6" spans="1:87">
+    <row r="6" spans="1:87" ht="14.4">
       <c r="A6" s="16">
         <v>2</v>
       </c>
@@ -3265,14 +3314,18 @@
       <c r="C7" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="26" t="s">
-        <v>33</v>
+      <c r="D7" s="95">
+        <v>43721</v>
       </c>
       <c r="E7" s="18">
-        <v>2</v>
-      </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
+        <v>2.5</v>
+      </c>
+      <c r="F7" s="114">
+        <v>43721.645833333336</v>
+      </c>
+      <c r="G7" s="114">
+        <v>43721.770833333336</v>
+      </c>
       <c r="H7" s="19" t="s">
         <v>30</v>
       </c>
@@ -3285,12 +3338,12 @@
       <c r="M7" s="23"/>
       <c r="N7" s="23"/>
       <c r="O7" s="28"/>
-      <c r="P7" s="28"/>
-      <c r="Q7" s="28"/>
-      <c r="R7" s="28"/>
-      <c r="S7" s="28"/>
-      <c r="T7" s="28"/>
-      <c r="U7" s="28"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="24"/>
+      <c r="S7" s="24"/>
+      <c r="T7" s="24"/>
+      <c r="U7" s="24"/>
       <c r="V7" s="24"/>
       <c r="W7" s="24"/>
       <c r="X7" s="24"/>
@@ -3365,14 +3418,18 @@
       <c r="C8" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="26" t="s">
-        <v>33</v>
+      <c r="D8" s="95">
+        <v>43721</v>
       </c>
       <c r="E8" s="18">
-        <v>1</v>
-      </c>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
+        <v>2.5</v>
+      </c>
+      <c r="F8" s="114">
+        <v>43721.645833333336</v>
+      </c>
+      <c r="G8" s="114">
+        <v>43721.770833333336</v>
+      </c>
       <c r="H8" s="19" t="s">
         <v>30</v>
       </c>
@@ -3383,12 +3440,12 @@
       <c r="M8" s="23"/>
       <c r="N8" s="23"/>
       <c r="O8" s="28"/>
-      <c r="P8" s="28"/>
-      <c r="Q8" s="28"/>
-      <c r="R8" s="28"/>
-      <c r="S8" s="28"/>
-      <c r="T8" s="28"/>
-      <c r="U8" s="28"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="24"/>
+      <c r="S8" s="24"/>
+      <c r="T8" s="24"/>
+      <c r="U8" s="24"/>
       <c r="V8" s="24"/>
       <c r="W8" s="24"/>
       <c r="X8" s="24"/>
@@ -3469,8 +3526,12 @@
       <c r="E9" s="18">
         <v>0.5</v>
       </c>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
+      <c r="F9" s="114">
+        <v>43721.645833333336</v>
+      </c>
+      <c r="G9" s="114">
+        <v>43721.770833333336</v>
+      </c>
       <c r="H9" s="19" t="s">
         <v>30</v>
       </c>
@@ -3481,12 +3542,12 @@
       <c r="M9" s="23"/>
       <c r="N9" s="23"/>
       <c r="O9" s="28"/>
-      <c r="P9" s="28"/>
-      <c r="Q9" s="28"/>
-      <c r="R9" s="28"/>
-      <c r="S9" s="28"/>
-      <c r="T9" s="28"/>
-      <c r="U9" s="28"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="24"/>
+      <c r="T9" s="24"/>
+      <c r="U9" s="24"/>
       <c r="V9" s="24"/>
       <c r="W9" s="24"/>
       <c r="X9" s="24"/>
@@ -3938,17 +3999,21 @@
       <c r="B14" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="33" t="s">
-        <v>38</v>
+      <c r="C14" s="95">
+        <v>43723</v>
+      </c>
+      <c r="D14" s="96">
+        <v>43723</v>
       </c>
       <c r="E14" s="34">
-        <v>1</v>
-      </c>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
+        <v>2</v>
+      </c>
+      <c r="F14" s="113">
+        <v>43723.458333333336</v>
+      </c>
+      <c r="G14" s="113">
+        <v>43723.520833333336</v>
+      </c>
       <c r="H14" s="32" t="s">
         <v>41</v>
       </c>
@@ -4046,7 +4111,7 @@
         <v>38</v>
       </c>
       <c r="E15" s="34">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F15" s="32"/>
       <c r="G15" s="32"/>
@@ -4133,7 +4198,7 @@
       <c r="CH15" s="40"/>
       <c r="CI15" s="40"/>
     </row>
-    <row r="16" spans="1:87" ht="43.2">
+    <row r="16" spans="1:87" ht="57.6">
       <c r="A16" s="16"/>
       <c r="B16" s="32" t="s">
         <v>44</v>
@@ -4145,10 +4210,14 @@
         <v>38</v>
       </c>
       <c r="E16" s="34">
-        <v>5</v>
-      </c>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
+        <v>2</v>
+      </c>
+      <c r="F16" s="113">
+        <v>43723.541666666664</v>
+      </c>
+      <c r="G16" s="113">
+        <v>43723.625</v>
+      </c>
       <c r="H16" s="32" t="s">
         <v>41</v>
       </c>
@@ -4236,29 +4305,29 @@
       <c r="CH16" s="40"/>
       <c r="CI16" s="40"/>
     </row>
-    <row r="17" spans="1:87" ht="14.4">
-      <c r="A17" s="16">
-        <v>4</v>
-      </c>
+    <row r="17" spans="1:87" s="94" customFormat="1" ht="14.4">
+      <c r="A17" s="16"/>
       <c r="B17" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
+        <v>131</v>
+      </c>
+      <c r="C17" s="115"/>
+      <c r="D17" s="34"/>
       <c r="E17" s="34"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
+      <c r="F17" s="113"/>
+      <c r="G17" s="113"/>
+      <c r="H17" s="32" t="s">
+        <v>41</v>
+      </c>
       <c r="I17" s="20"/>
       <c r="J17" s="20"/>
       <c r="K17" s="35"/>
       <c r="L17" s="36"/>
       <c r="M17" s="37"/>
       <c r="N17" s="37"/>
-      <c r="O17" s="37"/>
-      <c r="P17" s="37"/>
-      <c r="Q17" s="37"/>
-      <c r="R17" s="39"/>
+      <c r="O17" s="116"/>
+      <c r="P17" s="116"/>
+      <c r="Q17" s="116"/>
+      <c r="R17" s="116"/>
       <c r="S17" s="39"/>
       <c r="T17" s="39"/>
       <c r="U17" s="39"/>
@@ -4279,13 +4348,13 @@
       <c r="AJ17" s="39"/>
       <c r="AK17" s="39"/>
       <c r="AL17" s="39"/>
-      <c r="AM17" s="40"/>
-      <c r="AN17" s="40"/>
-      <c r="AO17" s="40"/>
-      <c r="AP17" s="40"/>
-      <c r="AQ17" s="40"/>
-      <c r="AR17" s="40"/>
-      <c r="AS17" s="40"/>
+      <c r="AM17" s="93"/>
+      <c r="AN17" s="93"/>
+      <c r="AO17" s="93"/>
+      <c r="AP17" s="93"/>
+      <c r="AQ17" s="93"/>
+      <c r="AR17" s="93"/>
+      <c r="AS17" s="93"/>
       <c r="AT17" s="39"/>
       <c r="AU17" s="39"/>
       <c r="AV17" s="39"/>
@@ -4293,13 +4362,13 @@
       <c r="AX17" s="39"/>
       <c r="AY17" s="39"/>
       <c r="AZ17" s="39"/>
-      <c r="BA17" s="40"/>
-      <c r="BB17" s="40"/>
-      <c r="BC17" s="40"/>
-      <c r="BD17" s="40"/>
-      <c r="BE17" s="40"/>
-      <c r="BF17" s="40"/>
-      <c r="BG17" s="40"/>
+      <c r="BA17" s="93"/>
+      <c r="BB17" s="93"/>
+      <c r="BC17" s="93"/>
+      <c r="BD17" s="93"/>
+      <c r="BE17" s="93"/>
+      <c r="BF17" s="93"/>
+      <c r="BG17" s="93"/>
       <c r="BH17" s="39"/>
       <c r="BI17" s="39"/>
       <c r="BJ17" s="39"/>
@@ -4321,33 +4390,27 @@
       <c r="BZ17" s="39"/>
       <c r="CA17" s="39"/>
       <c r="CB17" s="39"/>
-      <c r="CC17" s="40"/>
-      <c r="CD17" s="40"/>
-      <c r="CE17" s="40"/>
-      <c r="CF17" s="40"/>
-      <c r="CG17" s="40"/>
-      <c r="CH17" s="40"/>
-      <c r="CI17" s="40"/>
+      <c r="CC17" s="93"/>
+      <c r="CD17" s="93"/>
+      <c r="CE17" s="93"/>
+      <c r="CF17" s="93"/>
+      <c r="CG17" s="93"/>
+      <c r="CH17" s="93"/>
+      <c r="CI17" s="93"/>
     </row>
     <row r="18" spans="1:87" ht="14.4">
-      <c r="A18" s="16"/>
-      <c r="B18" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="111">
-        <v>43725</v>
-      </c>
-      <c r="D18" s="111">
-        <v>43728</v>
-      </c>
-      <c r="E18" s="34">
-        <v>2</v>
-      </c>
+      <c r="A18" s="16">
+        <v>4</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="34"/>
       <c r="F18" s="32"/>
       <c r="G18" s="32"/>
-      <c r="H18" s="32" t="s">
-        <v>30</v>
-      </c>
+      <c r="H18" s="32"/>
       <c r="I18" s="20"/>
       <c r="J18" s="20"/>
       <c r="K18" s="35"/>
@@ -4358,10 +4421,10 @@
       <c r="P18" s="37"/>
       <c r="Q18" s="37"/>
       <c r="R18" s="39"/>
-      <c r="S18" s="28"/>
-      <c r="T18" s="28"/>
-      <c r="U18" s="28"/>
-      <c r="V18" s="28"/>
+      <c r="S18" s="39"/>
+      <c r="T18" s="39"/>
+      <c r="U18" s="39"/>
+      <c r="V18" s="39"/>
       <c r="W18" s="39"/>
       <c r="X18" s="39"/>
       <c r="Y18" s="37"/>
@@ -4430,17 +4493,17 @@
     </row>
     <row r="19" spans="1:87" ht="14.4">
       <c r="A19" s="16"/>
-      <c r="B19" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="111">
+      <c r="B19" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="96">
         <v>43725</v>
       </c>
-      <c r="D19" s="111">
+      <c r="D19" s="96">
         <v>43728</v>
       </c>
       <c r="E19" s="34">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F19" s="32"/>
       <c r="G19" s="32"/>
@@ -4528,20 +4591,18 @@
       <c r="CI19" s="40"/>
     </row>
     <row r="20" spans="1:87" ht="14.4">
-      <c r="A20" s="16">
-        <v>5</v>
-      </c>
+      <c r="A20" s="16"/>
       <c r="B20" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="110">
-        <v>43726</v>
-      </c>
-      <c r="D20" s="110">
-        <v>43726</v>
+        <v>47</v>
+      </c>
+      <c r="C20" s="96">
+        <v>43725</v>
+      </c>
+      <c r="D20" s="96">
+        <v>43728</v>
       </c>
       <c r="E20" s="34">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F20" s="32"/>
       <c r="G20" s="32"/>
@@ -4558,10 +4619,10 @@
       <c r="P20" s="37"/>
       <c r="Q20" s="37"/>
       <c r="R20" s="39"/>
-      <c r="S20" s="39"/>
-      <c r="T20" s="38"/>
-      <c r="U20" s="39"/>
-      <c r="V20" s="39"/>
+      <c r="S20" s="28"/>
+      <c r="T20" s="28"/>
+      <c r="U20" s="28"/>
+      <c r="V20" s="28"/>
       <c r="W20" s="39"/>
       <c r="X20" s="39"/>
       <c r="Y20" s="37"/>
@@ -4628,196 +4689,204 @@
       <c r="CH20" s="40"/>
       <c r="CI20" s="40"/>
     </row>
-    <row r="21" spans="1:87">
-      <c r="A21" s="10" t="s">
+    <row r="21" spans="1:87" ht="14.4">
+      <c r="A21" s="16">
+        <v>5</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="95">
+        <v>43726</v>
+      </c>
+      <c r="D21" s="95">
+        <v>43726</v>
+      </c>
+      <c r="E21" s="34">
+        <v>3</v>
+      </c>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="37"/>
+      <c r="N21" s="37"/>
+      <c r="O21" s="37"/>
+      <c r="P21" s="37"/>
+      <c r="Q21" s="37"/>
+      <c r="R21" s="39"/>
+      <c r="S21" s="39"/>
+      <c r="T21" s="38"/>
+      <c r="U21" s="39"/>
+      <c r="V21" s="39"/>
+      <c r="W21" s="39"/>
+      <c r="X21" s="39"/>
+      <c r="Y21" s="37"/>
+      <c r="Z21" s="23"/>
+      <c r="AA21" s="23"/>
+      <c r="AB21" s="23"/>
+      <c r="AC21" s="37"/>
+      <c r="AD21" s="37"/>
+      <c r="AE21" s="37"/>
+      <c r="AF21" s="39"/>
+      <c r="AG21" s="39"/>
+      <c r="AH21" s="39"/>
+      <c r="AI21" s="39"/>
+      <c r="AJ21" s="39"/>
+      <c r="AK21" s="39"/>
+      <c r="AL21" s="39"/>
+      <c r="AM21" s="40"/>
+      <c r="AN21" s="40"/>
+      <c r="AO21" s="40"/>
+      <c r="AP21" s="40"/>
+      <c r="AQ21" s="40"/>
+      <c r="AR21" s="40"/>
+      <c r="AS21" s="40"/>
+      <c r="AT21" s="39"/>
+      <c r="AU21" s="39"/>
+      <c r="AV21" s="39"/>
+      <c r="AW21" s="39"/>
+      <c r="AX21" s="39"/>
+      <c r="AY21" s="39"/>
+      <c r="AZ21" s="39"/>
+      <c r="BA21" s="40"/>
+      <c r="BB21" s="40"/>
+      <c r="BC21" s="40"/>
+      <c r="BD21" s="40"/>
+      <c r="BE21" s="40"/>
+      <c r="BF21" s="40"/>
+      <c r="BG21" s="40"/>
+      <c r="BH21" s="39"/>
+      <c r="BI21" s="39"/>
+      <c r="BJ21" s="39"/>
+      <c r="BK21" s="39"/>
+      <c r="BL21" s="39"/>
+      <c r="BM21" s="39"/>
+      <c r="BN21" s="39"/>
+      <c r="BO21" s="37"/>
+      <c r="BP21" s="37"/>
+      <c r="BQ21" s="37"/>
+      <c r="BR21" s="37"/>
+      <c r="BS21" s="37"/>
+      <c r="BT21" s="37"/>
+      <c r="BU21" s="37"/>
+      <c r="BV21" s="39"/>
+      <c r="BW21" s="39"/>
+      <c r="BX21" s="39"/>
+      <c r="BY21" s="39"/>
+      <c r="BZ21" s="39"/>
+      <c r="CA21" s="39"/>
+      <c r="CB21" s="39"/>
+      <c r="CC21" s="40"/>
+      <c r="CD21" s="40"/>
+      <c r="CE21" s="40"/>
+      <c r="CF21" s="40"/>
+      <c r="CG21" s="40"/>
+      <c r="CH21" s="40"/>
+      <c r="CI21" s="40"/>
+    </row>
+    <row r="22" spans="1:87" ht="15.6">
+      <c r="A22" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="104"/>
-      <c r="D21" s="103"/>
-      <c r="E21" s="103"/>
-      <c r="F21" s="103"/>
-      <c r="G21" s="103"/>
-      <c r="H21" s="103"/>
-      <c r="I21" s="103"/>
-      <c r="J21" s="44"/>
-      <c r="K21" s="45"/>
-      <c r="L21" s="46"/>
-      <c r="M21" s="47"/>
-      <c r="N21" s="47"/>
-      <c r="O21" s="48"/>
-      <c r="P21" s="48"/>
-      <c r="Q21" s="48"/>
-      <c r="R21" s="48"/>
-      <c r="S21" s="48"/>
-      <c r="T21" s="48"/>
-      <c r="U21" s="48"/>
-      <c r="V21" s="48"/>
-      <c r="W21" s="48"/>
-      <c r="X21" s="48"/>
-      <c r="Y21" s="48"/>
-      <c r="Z21" s="48"/>
-      <c r="AA21" s="48"/>
-      <c r="AB21" s="48"/>
-      <c r="AC21" s="48"/>
-      <c r="AD21" s="48"/>
-      <c r="AE21" s="48"/>
-      <c r="AF21" s="48"/>
-      <c r="AG21" s="48"/>
-      <c r="AH21" s="48"/>
-      <c r="AI21" s="48"/>
-      <c r="AJ21" s="48"/>
-      <c r="AK21" s="48"/>
-      <c r="AL21" s="48"/>
-      <c r="AM21" s="48"/>
-      <c r="AN21" s="48"/>
-      <c r="AO21" s="48"/>
-      <c r="AP21" s="48"/>
-      <c r="AQ21" s="48"/>
-      <c r="AR21" s="48"/>
-      <c r="AS21" s="48"/>
-      <c r="AT21" s="48"/>
-      <c r="AU21" s="48"/>
-      <c r="AV21" s="48"/>
-      <c r="AW21" s="48"/>
-      <c r="AX21" s="48"/>
-      <c r="AY21" s="48"/>
-      <c r="AZ21" s="48"/>
-      <c r="BA21" s="48"/>
-      <c r="BB21" s="48"/>
-      <c r="BC21" s="48"/>
-      <c r="BD21" s="48"/>
-      <c r="BE21" s="48"/>
-      <c r="BF21" s="48"/>
-      <c r="BG21" s="48"/>
-      <c r="BH21" s="48"/>
-      <c r="BI21" s="48"/>
-      <c r="BJ21" s="48"/>
-      <c r="BK21" s="48"/>
-      <c r="BL21" s="48"/>
-      <c r="BM21" s="48"/>
-      <c r="BN21" s="48"/>
-      <c r="BO21" s="48"/>
-      <c r="BP21" s="48"/>
-      <c r="BQ21" s="48"/>
-      <c r="BR21" s="48"/>
-      <c r="BS21" s="48"/>
-      <c r="BT21" s="48"/>
-      <c r="BU21" s="48"/>
-      <c r="BV21" s="48"/>
-      <c r="BW21" s="48"/>
-      <c r="BX21" s="48"/>
-      <c r="BY21" s="48"/>
-      <c r="BZ21" s="48"/>
-      <c r="CA21" s="48"/>
-      <c r="CB21" s="48"/>
-      <c r="CC21" s="48"/>
-      <c r="CD21" s="48"/>
-      <c r="CE21" s="48"/>
-      <c r="CF21" s="48"/>
-      <c r="CG21" s="48"/>
-      <c r="CH21" s="48"/>
-      <c r="CI21" s="48"/>
-    </row>
-    <row r="22" spans="1:87" ht="28.8">
-      <c r="A22" s="16">
+      <c r="B22" s="43"/>
+      <c r="C22" s="101"/>
+      <c r="D22" s="98"/>
+      <c r="E22" s="98"/>
+      <c r="F22" s="98"/>
+      <c r="G22" s="98"/>
+      <c r="H22" s="98"/>
+      <c r="I22" s="98"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="45"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="47"/>
+      <c r="N22" s="47"/>
+      <c r="O22" s="48"/>
+      <c r="P22" s="48"/>
+      <c r="Q22" s="48"/>
+      <c r="R22" s="48"/>
+      <c r="S22" s="48"/>
+      <c r="T22" s="48"/>
+      <c r="U22" s="48"/>
+      <c r="V22" s="48"/>
+      <c r="W22" s="48"/>
+      <c r="X22" s="48"/>
+      <c r="Y22" s="48"/>
+      <c r="Z22" s="48"/>
+      <c r="AA22" s="48"/>
+      <c r="AB22" s="48"/>
+      <c r="AC22" s="48"/>
+      <c r="AD22" s="48"/>
+      <c r="AE22" s="48"/>
+      <c r="AF22" s="48"/>
+      <c r="AG22" s="48"/>
+      <c r="AH22" s="48"/>
+      <c r="AI22" s="48"/>
+      <c r="AJ22" s="48"/>
+      <c r="AK22" s="48"/>
+      <c r="AL22" s="48"/>
+      <c r="AM22" s="48"/>
+      <c r="AN22" s="48"/>
+      <c r="AO22" s="48"/>
+      <c r="AP22" s="48"/>
+      <c r="AQ22" s="48"/>
+      <c r="AR22" s="48"/>
+      <c r="AS22" s="48"/>
+      <c r="AT22" s="48"/>
+      <c r="AU22" s="48"/>
+      <c r="AV22" s="48"/>
+      <c r="AW22" s="48"/>
+      <c r="AX22" s="48"/>
+      <c r="AY22" s="48"/>
+      <c r="AZ22" s="48"/>
+      <c r="BA22" s="48"/>
+      <c r="BB22" s="48"/>
+      <c r="BC22" s="48"/>
+      <c r="BD22" s="48"/>
+      <c r="BE22" s="48"/>
+      <c r="BF22" s="48"/>
+      <c r="BG22" s="48"/>
+      <c r="BH22" s="48"/>
+      <c r="BI22" s="48"/>
+      <c r="BJ22" s="48"/>
+      <c r="BK22" s="48"/>
+      <c r="BL22" s="48"/>
+      <c r="BM22" s="48"/>
+      <c r="BN22" s="48"/>
+      <c r="BO22" s="48"/>
+      <c r="BP22" s="48"/>
+      <c r="BQ22" s="48"/>
+      <c r="BR22" s="48"/>
+      <c r="BS22" s="48"/>
+      <c r="BT22" s="48"/>
+      <c r="BU22" s="48"/>
+      <c r="BV22" s="48"/>
+      <c r="BW22" s="48"/>
+      <c r="BX22" s="48"/>
+      <c r="BY22" s="48"/>
+      <c r="BZ22" s="48"/>
+      <c r="CA22" s="48"/>
+      <c r="CB22" s="48"/>
+      <c r="CC22" s="48"/>
+      <c r="CD22" s="48"/>
+      <c r="CE22" s="48"/>
+      <c r="CF22" s="48"/>
+      <c r="CG22" s="48"/>
+      <c r="CH22" s="48"/>
+      <c r="CI22" s="48"/>
+    </row>
+    <row r="23" spans="1:87" ht="28.8">
+      <c r="A23" s="16">
         <v>1</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B23" s="19" t="s">
         <v>50</v>
-      </c>
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="23"/>
-      <c r="N22" s="23"/>
-      <c r="O22" s="23"/>
-      <c r="P22" s="23"/>
-      <c r="Q22" s="23"/>
-      <c r="R22" s="24"/>
-      <c r="S22" s="24"/>
-      <c r="T22" s="24"/>
-      <c r="U22" s="24"/>
-      <c r="V22" s="24"/>
-      <c r="W22" s="24"/>
-      <c r="X22" s="24"/>
-      <c r="Y22" s="23"/>
-      <c r="Z22" s="23"/>
-      <c r="AA22" s="23"/>
-      <c r="AB22" s="23"/>
-      <c r="AC22" s="23"/>
-      <c r="AD22" s="23"/>
-      <c r="AE22" s="23"/>
-      <c r="AF22" s="24"/>
-      <c r="AG22" s="24"/>
-      <c r="AH22" s="24"/>
-      <c r="AI22" s="24"/>
-      <c r="AJ22" s="24"/>
-      <c r="AK22" s="24"/>
-      <c r="AL22" s="24"/>
-      <c r="AM22" s="25"/>
-      <c r="AN22" s="25"/>
-      <c r="AO22" s="25"/>
-      <c r="AP22" s="25"/>
-      <c r="AQ22" s="25"/>
-      <c r="AR22" s="25"/>
-      <c r="AS22" s="25"/>
-      <c r="AT22" s="24"/>
-      <c r="AU22" s="24"/>
-      <c r="AV22" s="24"/>
-      <c r="AW22" s="24"/>
-      <c r="AX22" s="24"/>
-      <c r="AY22" s="24"/>
-      <c r="AZ22" s="24"/>
-      <c r="BA22" s="25"/>
-      <c r="BB22" s="25"/>
-      <c r="BC22" s="25"/>
-      <c r="BD22" s="25"/>
-      <c r="BE22" s="25"/>
-      <c r="BF22" s="25"/>
-      <c r="BG22" s="25"/>
-      <c r="BH22" s="24"/>
-      <c r="BI22" s="24"/>
-      <c r="BJ22" s="24"/>
-      <c r="BK22" s="24"/>
-      <c r="BL22" s="24"/>
-      <c r="BM22" s="24"/>
-      <c r="BN22" s="24"/>
-      <c r="BO22" s="23"/>
-      <c r="BP22" s="23"/>
-      <c r="BQ22" s="23"/>
-      <c r="BR22" s="23"/>
-      <c r="BS22" s="23"/>
-      <c r="BT22" s="23"/>
-      <c r="BU22" s="23"/>
-      <c r="BV22" s="24"/>
-      <c r="BW22" s="24"/>
-      <c r="BX22" s="24"/>
-      <c r="BY22" s="24"/>
-      <c r="BZ22" s="24"/>
-      <c r="CA22" s="24"/>
-      <c r="CB22" s="24"/>
-      <c r="CC22" s="25"/>
-      <c r="CD22" s="25"/>
-      <c r="CE22" s="25"/>
-      <c r="CF22" s="25"/>
-      <c r="CG22" s="25"/>
-      <c r="CH22" s="25"/>
-      <c r="CI22" s="25"/>
-    </row>
-    <row r="23" spans="1:87" ht="14.4">
-      <c r="A23" s="16">
-        <v>2</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>51</v>
       </c>
       <c r="C23" s="49"/>
       <c r="D23" s="49"/>
@@ -4905,10 +4974,12 @@
       <c r="CH23" s="25"/>
       <c r="CI23" s="25"/>
     </row>
-    <row r="24" spans="1:87" ht="28.8">
-      <c r="A24" s="16"/>
-      <c r="B24" s="19" t="s">
-        <v>52</v>
+    <row r="24" spans="1:87" ht="14.4">
+      <c r="A24" s="16">
+        <v>2</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>51</v>
       </c>
       <c r="C24" s="49"/>
       <c r="D24" s="49"/>
@@ -4916,8 +4987,8 @@
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
       <c r="H24" s="19"/>
-      <c r="I24" s="50"/>
-      <c r="J24" s="51"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="20"/>
       <c r="K24" s="21"/>
       <c r="L24" s="22"/>
       <c r="M24" s="23"/>
@@ -4999,7 +5070,7 @@
     <row r="25" spans="1:87" ht="28.8">
       <c r="A25" s="16"/>
       <c r="B25" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C25" s="49"/>
       <c r="D25" s="49"/>
@@ -5087,10 +5158,10 @@
       <c r="CH25" s="25"/>
       <c r="CI25" s="25"/>
     </row>
-    <row r="26" spans="1:87" ht="14.4">
+    <row r="26" spans="1:87" ht="28.8">
       <c r="A26" s="16"/>
       <c r="B26" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C26" s="49"/>
       <c r="D26" s="49"/>
@@ -5178,10 +5249,10 @@
       <c r="CH26" s="25"/>
       <c r="CI26" s="25"/>
     </row>
-    <row r="27" spans="1:87" ht="28.8">
+    <row r="27" spans="1:87" ht="14.4">
       <c r="A27" s="16"/>
       <c r="B27" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C27" s="49"/>
       <c r="D27" s="49"/>
@@ -5269,12 +5340,10 @@
       <c r="CH27" s="25"/>
       <c r="CI27" s="25"/>
     </row>
-    <row r="28" spans="1:87" ht="14.4">
-      <c r="A28" s="16" t="s">
-        <v>56</v>
-      </c>
+    <row r="28" spans="1:87" ht="28.8">
+      <c r="A28" s="16"/>
       <c r="B28" s="19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C28" s="49"/>
       <c r="D28" s="49"/>
@@ -5302,7 +5371,7 @@
       <c r="Z28" s="23"/>
       <c r="AA28" s="23"/>
       <c r="AB28" s="23"/>
-      <c r="AC28" s="52"/>
+      <c r="AC28" s="23"/>
       <c r="AD28" s="23"/>
       <c r="AE28" s="23"/>
       <c r="AF28" s="24"/>
@@ -5362,193 +5431,196 @@
       <c r="CH28" s="25"/>
       <c r="CI28" s="25"/>
     </row>
-    <row r="29" spans="1:87">
-      <c r="A29" s="10" t="s">
+    <row r="29" spans="1:87" ht="14.4">
+      <c r="A29" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="51"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="23"/>
+      <c r="Q29" s="23"/>
+      <c r="R29" s="24"/>
+      <c r="S29" s="24"/>
+      <c r="T29" s="24"/>
+      <c r="U29" s="24"/>
+      <c r="V29" s="24"/>
+      <c r="W29" s="24"/>
+      <c r="X29" s="24"/>
+      <c r="Y29" s="23"/>
+      <c r="Z29" s="23"/>
+      <c r="AA29" s="23"/>
+      <c r="AB29" s="23"/>
+      <c r="AC29" s="52"/>
+      <c r="AD29" s="23"/>
+      <c r="AE29" s="23"/>
+      <c r="AF29" s="24"/>
+      <c r="AG29" s="24"/>
+      <c r="AH29" s="24"/>
+      <c r="AI29" s="24"/>
+      <c r="AJ29" s="24"/>
+      <c r="AK29" s="24"/>
+      <c r="AL29" s="24"/>
+      <c r="AM29" s="25"/>
+      <c r="AN29" s="25"/>
+      <c r="AO29" s="25"/>
+      <c r="AP29" s="25"/>
+      <c r="AQ29" s="25"/>
+      <c r="AR29" s="25"/>
+      <c r="AS29" s="25"/>
+      <c r="AT29" s="24"/>
+      <c r="AU29" s="24"/>
+      <c r="AV29" s="24"/>
+      <c r="AW29" s="24"/>
+      <c r="AX29" s="24"/>
+      <c r="AY29" s="24"/>
+      <c r="AZ29" s="24"/>
+      <c r="BA29" s="25"/>
+      <c r="BB29" s="25"/>
+      <c r="BC29" s="25"/>
+      <c r="BD29" s="25"/>
+      <c r="BE29" s="25"/>
+      <c r="BF29" s="25"/>
+      <c r="BG29" s="25"/>
+      <c r="BH29" s="24"/>
+      <c r="BI29" s="24"/>
+      <c r="BJ29" s="24"/>
+      <c r="BK29" s="24"/>
+      <c r="BL29" s="24"/>
+      <c r="BM29" s="24"/>
+      <c r="BN29" s="24"/>
+      <c r="BO29" s="23"/>
+      <c r="BP29" s="23"/>
+      <c r="BQ29" s="23"/>
+      <c r="BR29" s="23"/>
+      <c r="BS29" s="23"/>
+      <c r="BT29" s="23"/>
+      <c r="BU29" s="23"/>
+      <c r="BV29" s="24"/>
+      <c r="BW29" s="24"/>
+      <c r="BX29" s="24"/>
+      <c r="BY29" s="24"/>
+      <c r="BZ29" s="24"/>
+      <c r="CA29" s="24"/>
+      <c r="CB29" s="24"/>
+      <c r="CC29" s="25"/>
+      <c r="CD29" s="25"/>
+      <c r="CE29" s="25"/>
+      <c r="CF29" s="25"/>
+      <c r="CG29" s="25"/>
+      <c r="CH29" s="25"/>
+      <c r="CI29" s="25"/>
+    </row>
+    <row r="30" spans="1:87" ht="15.6">
+      <c r="A30" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="44"/>
-      <c r="K29" s="45"/>
-      <c r="L29" s="46"/>
-      <c r="M29" s="47"/>
-      <c r="N29" s="47"/>
-      <c r="O29" s="48"/>
-      <c r="P29" s="48"/>
-      <c r="Q29" s="48"/>
-      <c r="R29" s="53"/>
-      <c r="S29" s="53"/>
-      <c r="T29" s="53"/>
-      <c r="U29" s="53"/>
-      <c r="V29" s="53"/>
-      <c r="W29" s="48"/>
-      <c r="X29" s="48"/>
-      <c r="Y29" s="48"/>
-      <c r="Z29" s="48"/>
-      <c r="AA29" s="48"/>
-      <c r="AB29" s="48"/>
-      <c r="AC29" s="48"/>
-      <c r="AD29" s="48"/>
-      <c r="AE29" s="48"/>
-      <c r="AF29" s="48"/>
-      <c r="AG29" s="48"/>
-      <c r="AH29" s="48"/>
-      <c r="AI29" s="48"/>
-      <c r="AJ29" s="48"/>
-      <c r="AK29" s="48"/>
-      <c r="AL29" s="48"/>
-      <c r="AM29" s="48"/>
-      <c r="AN29" s="48"/>
-      <c r="AO29" s="48"/>
-      <c r="AP29" s="48"/>
-      <c r="AQ29" s="48"/>
-      <c r="AR29" s="48"/>
-      <c r="AS29" s="48"/>
-      <c r="AT29" s="48"/>
-      <c r="AU29" s="48"/>
-      <c r="AV29" s="48"/>
-      <c r="AW29" s="48"/>
-      <c r="AX29" s="48"/>
-      <c r="AY29" s="48"/>
-      <c r="AZ29" s="48"/>
-      <c r="BA29" s="48"/>
-      <c r="BB29" s="48"/>
-      <c r="BC29" s="48"/>
-      <c r="BD29" s="48"/>
-      <c r="BE29" s="48"/>
-      <c r="BF29" s="48"/>
-      <c r="BG29" s="48"/>
-      <c r="BH29" s="48"/>
-      <c r="BI29" s="48"/>
-      <c r="BJ29" s="48"/>
-      <c r="BK29" s="48"/>
-      <c r="BL29" s="48"/>
-      <c r="BM29" s="48"/>
-      <c r="BN29" s="48"/>
-      <c r="BO29" s="48"/>
-      <c r="BP29" s="48"/>
-      <c r="BQ29" s="48"/>
-      <c r="BR29" s="48"/>
-      <c r="BS29" s="48"/>
-      <c r="BT29" s="48"/>
-      <c r="BU29" s="48"/>
-      <c r="BV29" s="48"/>
-      <c r="BW29" s="48"/>
-      <c r="BX29" s="48"/>
-      <c r="BY29" s="48"/>
-      <c r="BZ29" s="48"/>
-      <c r="CA29" s="48"/>
-      <c r="CB29" s="48"/>
-      <c r="CC29" s="48"/>
-      <c r="CD29" s="48"/>
-      <c r="CE29" s="48"/>
-      <c r="CF29" s="48"/>
-      <c r="CG29" s="48"/>
-      <c r="CH29" s="48"/>
-      <c r="CI29" s="48"/>
-    </row>
-    <row r="30" spans="1:87">
-      <c r="A30" s="16">
+      <c r="B30" s="43"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="43"/>
+      <c r="J30" s="44"/>
+      <c r="K30" s="45"/>
+      <c r="L30" s="46"/>
+      <c r="M30" s="47"/>
+      <c r="N30" s="47"/>
+      <c r="O30" s="48"/>
+      <c r="P30" s="48"/>
+      <c r="Q30" s="48"/>
+      <c r="R30" s="53"/>
+      <c r="S30" s="53"/>
+      <c r="T30" s="53"/>
+      <c r="U30" s="53"/>
+      <c r="V30" s="53"/>
+      <c r="W30" s="48"/>
+      <c r="X30" s="48"/>
+      <c r="Y30" s="48"/>
+      <c r="Z30" s="48"/>
+      <c r="AA30" s="48"/>
+      <c r="AB30" s="48"/>
+      <c r="AC30" s="48"/>
+      <c r="AD30" s="48"/>
+      <c r="AE30" s="48"/>
+      <c r="AF30" s="48"/>
+      <c r="AG30" s="48"/>
+      <c r="AH30" s="48"/>
+      <c r="AI30" s="48"/>
+      <c r="AJ30" s="48"/>
+      <c r="AK30" s="48"/>
+      <c r="AL30" s="48"/>
+      <c r="AM30" s="48"/>
+      <c r="AN30" s="48"/>
+      <c r="AO30" s="48"/>
+      <c r="AP30" s="48"/>
+      <c r="AQ30" s="48"/>
+      <c r="AR30" s="48"/>
+      <c r="AS30" s="48"/>
+      <c r="AT30" s="48"/>
+      <c r="AU30" s="48"/>
+      <c r="AV30" s="48"/>
+      <c r="AW30" s="48"/>
+      <c r="AX30" s="48"/>
+      <c r="AY30" s="48"/>
+      <c r="AZ30" s="48"/>
+      <c r="BA30" s="48"/>
+      <c r="BB30" s="48"/>
+      <c r="BC30" s="48"/>
+      <c r="BD30" s="48"/>
+      <c r="BE30" s="48"/>
+      <c r="BF30" s="48"/>
+      <c r="BG30" s="48"/>
+      <c r="BH30" s="48"/>
+      <c r="BI30" s="48"/>
+      <c r="BJ30" s="48"/>
+      <c r="BK30" s="48"/>
+      <c r="BL30" s="48"/>
+      <c r="BM30" s="48"/>
+      <c r="BN30" s="48"/>
+      <c r="BO30" s="48"/>
+      <c r="BP30" s="48"/>
+      <c r="BQ30" s="48"/>
+      <c r="BR30" s="48"/>
+      <c r="BS30" s="48"/>
+      <c r="BT30" s="48"/>
+      <c r="BU30" s="48"/>
+      <c r="BV30" s="48"/>
+      <c r="BW30" s="48"/>
+      <c r="BX30" s="48"/>
+      <c r="BY30" s="48"/>
+      <c r="BZ30" s="48"/>
+      <c r="CA30" s="48"/>
+      <c r="CB30" s="48"/>
+      <c r="CC30" s="48"/>
+      <c r="CD30" s="48"/>
+      <c r="CE30" s="48"/>
+      <c r="CF30" s="48"/>
+      <c r="CG30" s="48"/>
+      <c r="CH30" s="48"/>
+      <c r="CI30" s="48"/>
+    </row>
+    <row r="31" spans="1:87" ht="14.4">
+      <c r="A31" s="16">
         <v>1</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="B31" s="19" t="s">
         <v>59</v>
-      </c>
-      <c r="C30" s="49"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="50"/>
-      <c r="J30" s="51"/>
-      <c r="K30" s="21"/>
-      <c r="L30" s="22"/>
-      <c r="M30" s="23"/>
-      <c r="N30" s="23"/>
-      <c r="O30" s="23"/>
-      <c r="P30" s="23"/>
-      <c r="Q30" s="23"/>
-      <c r="R30" s="24"/>
-      <c r="S30" s="24"/>
-      <c r="T30" s="24"/>
-      <c r="U30" s="24"/>
-      <c r="V30" s="24"/>
-      <c r="W30" s="24"/>
-      <c r="X30" s="24"/>
-      <c r="Y30" s="23"/>
-      <c r="Z30" s="23"/>
-      <c r="AA30" s="23"/>
-      <c r="AB30" s="23"/>
-      <c r="AC30" s="23"/>
-      <c r="AD30" s="23"/>
-      <c r="AE30" s="23"/>
-      <c r="AF30" s="24"/>
-      <c r="AG30" s="24"/>
-      <c r="AH30" s="24"/>
-      <c r="AI30" s="24"/>
-      <c r="AJ30" s="24"/>
-      <c r="AK30" s="24"/>
-      <c r="AL30" s="24"/>
-      <c r="AM30" s="25"/>
-      <c r="AN30" s="25"/>
-      <c r="AO30" s="25"/>
-      <c r="AP30" s="25"/>
-      <c r="AQ30" s="25"/>
-      <c r="AR30" s="25"/>
-      <c r="AS30" s="25"/>
-      <c r="AT30" s="24"/>
-      <c r="AU30" s="24"/>
-      <c r="AV30" s="24"/>
-      <c r="AW30" s="24"/>
-      <c r="AX30" s="24"/>
-      <c r="AY30" s="24"/>
-      <c r="AZ30" s="24"/>
-      <c r="BA30" s="25"/>
-      <c r="BB30" s="25"/>
-      <c r="BC30" s="25"/>
-      <c r="BD30" s="25"/>
-      <c r="BE30" s="25"/>
-      <c r="BF30" s="25"/>
-      <c r="BG30" s="25"/>
-      <c r="BH30" s="24"/>
-      <c r="BI30" s="24"/>
-      <c r="BJ30" s="24"/>
-      <c r="BK30" s="24"/>
-      <c r="BL30" s="24"/>
-      <c r="BM30" s="24"/>
-      <c r="BN30" s="24"/>
-      <c r="BO30" s="23"/>
-      <c r="BP30" s="23"/>
-      <c r="BQ30" s="23"/>
-      <c r="BR30" s="23"/>
-      <c r="BS30" s="23"/>
-      <c r="BT30" s="23"/>
-      <c r="BU30" s="23"/>
-      <c r="BV30" s="24"/>
-      <c r="BW30" s="24"/>
-      <c r="BX30" s="24"/>
-      <c r="BY30" s="24"/>
-      <c r="BZ30" s="24"/>
-      <c r="CA30" s="24"/>
-      <c r="CB30" s="24"/>
-      <c r="CC30" s="25"/>
-      <c r="CD30" s="25"/>
-      <c r="CE30" s="25"/>
-      <c r="CF30" s="25"/>
-      <c r="CG30" s="25"/>
-      <c r="CH30" s="25"/>
-      <c r="CI30" s="25"/>
-    </row>
-    <row r="31" spans="1:87">
-      <c r="B31" s="17" t="s">
-        <v>60</v>
       </c>
       <c r="C31" s="49"/>
       <c r="D31" s="49"/>
@@ -5636,9 +5708,9 @@
       <c r="CH31" s="25"/>
       <c r="CI31" s="25"/>
     </row>
-    <row r="32" spans="1:87">
+    <row r="32" spans="1:87" ht="28.8">
       <c r="B32" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C32" s="49"/>
       <c r="D32" s="49"/>
@@ -5726,12 +5798,9 @@
       <c r="CH32" s="25"/>
       <c r="CI32" s="25"/>
     </row>
-    <row r="33" spans="1:87">
-      <c r="A33" s="16">
-        <v>2</v>
-      </c>
-      <c r="B33" s="19" t="s">
-        <v>62</v>
+    <row r="33" spans="1:87" ht="14.4">
+      <c r="B33" s="17" t="s">
+        <v>61</v>
       </c>
       <c r="C33" s="49"/>
       <c r="D33" s="49"/>
@@ -5819,10 +5888,12 @@
       <c r="CH33" s="25"/>
       <c r="CI33" s="25"/>
     </row>
-    <row r="34" spans="1:87">
-      <c r="A34" s="16"/>
+    <row r="34" spans="1:87" ht="14.4">
+      <c r="A34" s="16">
+        <v>2</v>
+      </c>
       <c r="B34" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C34" s="49"/>
       <c r="D34" s="49"/>
@@ -5910,10 +5981,10 @@
       <c r="CH34" s="25"/>
       <c r="CI34" s="25"/>
     </row>
-    <row r="35" spans="1:87">
+    <row r="35" spans="1:87" ht="14.4">
       <c r="A35" s="16"/>
       <c r="B35" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C35" s="49"/>
       <c r="D35" s="49"/>
@@ -6001,10 +6072,10 @@
       <c r="CH35" s="25"/>
       <c r="CI35" s="25"/>
     </row>
-    <row r="36" spans="1:87">
+    <row r="36" spans="1:87" ht="14.4">
       <c r="A36" s="16"/>
-      <c r="B36" s="54" t="s">
-        <v>65</v>
+      <c r="B36" s="19" t="s">
+        <v>64</v>
       </c>
       <c r="C36" s="49"/>
       <c r="D36" s="49"/>
@@ -6092,10 +6163,10 @@
       <c r="CH36" s="25"/>
       <c r="CI36" s="25"/>
     </row>
-    <row r="37" spans="1:87">
+    <row r="37" spans="1:87" ht="14.4">
       <c r="A37" s="16"/>
-      <c r="B37" s="19" t="s">
-        <v>66</v>
+      <c r="B37" s="54" t="s">
+        <v>65</v>
       </c>
       <c r="C37" s="49"/>
       <c r="D37" s="49"/>
@@ -6183,10 +6254,10 @@
       <c r="CH37" s="25"/>
       <c r="CI37" s="25"/>
     </row>
-    <row r="38" spans="1:87">
+    <row r="38" spans="1:87" ht="14.4">
       <c r="A38" s="16"/>
       <c r="B38" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C38" s="49"/>
       <c r="D38" s="49"/>
@@ -6274,10 +6345,10 @@
       <c r="CH38" s="25"/>
       <c r="CI38" s="25"/>
     </row>
-    <row r="39" spans="1:87">
+    <row r="39" spans="1:87" ht="14.4">
       <c r="A39" s="16"/>
       <c r="B39" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C39" s="49"/>
       <c r="D39" s="49"/>
@@ -6365,10 +6436,10 @@
       <c r="CH39" s="25"/>
       <c r="CI39" s="25"/>
     </row>
-    <row r="40" spans="1:87">
+    <row r="40" spans="1:87" ht="14.4">
       <c r="A40" s="16"/>
       <c r="B40" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C40" s="49"/>
       <c r="D40" s="49"/>
@@ -6456,10 +6527,10 @@
       <c r="CH40" s="25"/>
       <c r="CI40" s="25"/>
     </row>
-    <row r="41" spans="1:87">
+    <row r="41" spans="1:87" ht="14.4">
       <c r="A41" s="16"/>
       <c r="B41" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C41" s="49"/>
       <c r="D41" s="49"/>
@@ -6547,10 +6618,10 @@
       <c r="CH41" s="25"/>
       <c r="CI41" s="25"/>
     </row>
-    <row r="42" spans="1:87">
+    <row r="42" spans="1:87" ht="14.4">
       <c r="A42" s="16"/>
       <c r="B42" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C42" s="49"/>
       <c r="D42" s="49"/>
@@ -6638,9 +6709,10 @@
       <c r="CH42" s="25"/>
       <c r="CI42" s="25"/>
     </row>
-    <row r="43" spans="1:87">
+    <row r="43" spans="1:87" ht="14.4">
+      <c r="A43" s="16"/>
       <c r="B43" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C43" s="49"/>
       <c r="D43" s="49"/>
@@ -6728,12 +6800,9 @@
       <c r="CH43" s="25"/>
       <c r="CI43" s="25"/>
     </row>
-    <row r="44" spans="1:87">
-      <c r="A44" s="16" t="s">
-        <v>56</v>
-      </c>
+    <row r="44" spans="1:87" ht="14.4">
       <c r="B44" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C44" s="49"/>
       <c r="D44" s="49"/>
@@ -6782,7 +6851,7 @@
       <c r="AU44" s="24"/>
       <c r="AV44" s="24"/>
       <c r="AW44" s="24"/>
-      <c r="AX44" s="52"/>
+      <c r="AX44" s="24"/>
       <c r="AY44" s="24"/>
       <c r="AZ44" s="24"/>
       <c r="BA44" s="25"/>
@@ -6821,196 +6890,196 @@
       <c r="CH44" s="25"/>
       <c r="CI44" s="25"/>
     </row>
-    <row r="45" spans="1:87">
-      <c r="A45" s="10" t="s">
+    <row r="45" spans="1:87" ht="14.4">
+      <c r="A45" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C45" s="49"/>
+      <c r="D45" s="49"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="19"/>
+      <c r="I45" s="50"/>
+      <c r="J45" s="51"/>
+      <c r="K45" s="21"/>
+      <c r="L45" s="22"/>
+      <c r="M45" s="23"/>
+      <c r="N45" s="23"/>
+      <c r="O45" s="23"/>
+      <c r="P45" s="23"/>
+      <c r="Q45" s="23"/>
+      <c r="R45" s="24"/>
+      <c r="S45" s="24"/>
+      <c r="T45" s="24"/>
+      <c r="U45" s="24"/>
+      <c r="V45" s="24"/>
+      <c r="W45" s="24"/>
+      <c r="X45" s="24"/>
+      <c r="Y45" s="23"/>
+      <c r="Z45" s="23"/>
+      <c r="AA45" s="23"/>
+      <c r="AB45" s="23"/>
+      <c r="AC45" s="23"/>
+      <c r="AD45" s="23"/>
+      <c r="AE45" s="23"/>
+      <c r="AF45" s="24"/>
+      <c r="AG45" s="24"/>
+      <c r="AH45" s="24"/>
+      <c r="AI45" s="24"/>
+      <c r="AJ45" s="24"/>
+      <c r="AK45" s="24"/>
+      <c r="AL45" s="24"/>
+      <c r="AM45" s="25"/>
+      <c r="AN45" s="25"/>
+      <c r="AO45" s="25"/>
+      <c r="AP45" s="25"/>
+      <c r="AQ45" s="25"/>
+      <c r="AR45" s="25"/>
+      <c r="AS45" s="25"/>
+      <c r="AT45" s="24"/>
+      <c r="AU45" s="24"/>
+      <c r="AV45" s="24"/>
+      <c r="AW45" s="24"/>
+      <c r="AX45" s="52"/>
+      <c r="AY45" s="24"/>
+      <c r="AZ45" s="24"/>
+      <c r="BA45" s="25"/>
+      <c r="BB45" s="25"/>
+      <c r="BC45" s="25"/>
+      <c r="BD45" s="25"/>
+      <c r="BE45" s="25"/>
+      <c r="BF45" s="25"/>
+      <c r="BG45" s="25"/>
+      <c r="BH45" s="24"/>
+      <c r="BI45" s="24"/>
+      <c r="BJ45" s="24"/>
+      <c r="BK45" s="24"/>
+      <c r="BL45" s="24"/>
+      <c r="BM45" s="24"/>
+      <c r="BN45" s="24"/>
+      <c r="BO45" s="23"/>
+      <c r="BP45" s="23"/>
+      <c r="BQ45" s="23"/>
+      <c r="BR45" s="23"/>
+      <c r="BS45" s="23"/>
+      <c r="BT45" s="23"/>
+      <c r="BU45" s="23"/>
+      <c r="BV45" s="24"/>
+      <c r="BW45" s="24"/>
+      <c r="BX45" s="24"/>
+      <c r="BY45" s="24"/>
+      <c r="BZ45" s="24"/>
+      <c r="CA45" s="24"/>
+      <c r="CB45" s="24"/>
+      <c r="CC45" s="25"/>
+      <c r="CD45" s="25"/>
+      <c r="CE45" s="25"/>
+      <c r="CF45" s="25"/>
+      <c r="CG45" s="25"/>
+      <c r="CH45" s="25"/>
+      <c r="CI45" s="25"/>
+    </row>
+    <row r="46" spans="1:87" ht="15.6">
+      <c r="A46" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B45" s="43"/>
-      <c r="C45" s="104"/>
-      <c r="D45" s="103"/>
-      <c r="E45" s="103"/>
-      <c r="F45" s="103"/>
-      <c r="G45" s="103"/>
-      <c r="H45" s="103"/>
-      <c r="I45" s="103"/>
-      <c r="J45" s="44"/>
-      <c r="K45" s="45"/>
-      <c r="L45" s="46"/>
-      <c r="M45" s="47"/>
-      <c r="N45" s="47"/>
-      <c r="O45" s="48"/>
-      <c r="P45" s="48"/>
-      <c r="Q45" s="48"/>
-      <c r="R45" s="48"/>
-      <c r="S45" s="48"/>
-      <c r="T45" s="48"/>
-      <c r="U45" s="48"/>
-      <c r="V45" s="48"/>
-      <c r="W45" s="48"/>
-      <c r="X45" s="48"/>
-      <c r="Y45" s="48"/>
-      <c r="Z45" s="48"/>
-      <c r="AA45" s="48"/>
-      <c r="AB45" s="48"/>
-      <c r="AC45" s="48"/>
-      <c r="AD45" s="48"/>
-      <c r="AE45" s="48"/>
-      <c r="AF45" s="48"/>
-      <c r="AG45" s="48"/>
-      <c r="AH45" s="48"/>
-      <c r="AI45" s="48"/>
-      <c r="AJ45" s="48"/>
-      <c r="AK45" s="48"/>
-      <c r="AL45" s="48"/>
-      <c r="AM45" s="48"/>
-      <c r="AN45" s="48"/>
-      <c r="AO45" s="48"/>
-      <c r="AP45" s="48"/>
-      <c r="AQ45" s="48"/>
-      <c r="AR45" s="48"/>
-      <c r="AS45" s="48"/>
-      <c r="AT45" s="48"/>
-      <c r="AU45" s="48"/>
-      <c r="AV45" s="48"/>
-      <c r="AW45" s="48"/>
-      <c r="AX45" s="48"/>
-      <c r="AY45" s="48"/>
-      <c r="AZ45" s="48"/>
-      <c r="BA45" s="48"/>
-      <c r="BB45" s="48"/>
-      <c r="BC45" s="48"/>
-      <c r="BD45" s="48"/>
-      <c r="BE45" s="48"/>
-      <c r="BF45" s="48"/>
-      <c r="BG45" s="48"/>
-      <c r="BH45" s="48"/>
-      <c r="BI45" s="48"/>
-      <c r="BJ45" s="48"/>
-      <c r="BK45" s="48"/>
-      <c r="BL45" s="48"/>
-      <c r="BM45" s="48"/>
-      <c r="BN45" s="48"/>
-      <c r="BO45" s="48"/>
-      <c r="BP45" s="48"/>
-      <c r="BQ45" s="48"/>
-      <c r="BR45" s="48"/>
-      <c r="BS45" s="48"/>
-      <c r="BT45" s="48"/>
-      <c r="BU45" s="48"/>
-      <c r="BV45" s="48"/>
-      <c r="BW45" s="48"/>
-      <c r="BX45" s="48"/>
-      <c r="BY45" s="48"/>
-      <c r="BZ45" s="48"/>
-      <c r="CA45" s="48"/>
-      <c r="CB45" s="48"/>
-      <c r="CC45" s="48"/>
-      <c r="CD45" s="48"/>
-      <c r="CE45" s="48"/>
-      <c r="CF45" s="48"/>
-      <c r="CG45" s="48"/>
-      <c r="CH45" s="48"/>
-      <c r="CI45" s="48"/>
-    </row>
-    <row r="46" spans="1:87">
-      <c r="A46" s="16">
+      <c r="B46" s="43"/>
+      <c r="C46" s="101"/>
+      <c r="D46" s="98"/>
+      <c r="E46" s="98"/>
+      <c r="F46" s="98"/>
+      <c r="G46" s="98"/>
+      <c r="H46" s="98"/>
+      <c r="I46" s="98"/>
+      <c r="J46" s="44"/>
+      <c r="K46" s="45"/>
+      <c r="L46" s="46"/>
+      <c r="M46" s="47"/>
+      <c r="N46" s="47"/>
+      <c r="O46" s="48"/>
+      <c r="P46" s="48"/>
+      <c r="Q46" s="48"/>
+      <c r="R46" s="48"/>
+      <c r="S46" s="48"/>
+      <c r="T46" s="48"/>
+      <c r="U46" s="48"/>
+      <c r="V46" s="48"/>
+      <c r="W46" s="48"/>
+      <c r="X46" s="48"/>
+      <c r="Y46" s="48"/>
+      <c r="Z46" s="48"/>
+      <c r="AA46" s="48"/>
+      <c r="AB46" s="48"/>
+      <c r="AC46" s="48"/>
+      <c r="AD46" s="48"/>
+      <c r="AE46" s="48"/>
+      <c r="AF46" s="48"/>
+      <c r="AG46" s="48"/>
+      <c r="AH46" s="48"/>
+      <c r="AI46" s="48"/>
+      <c r="AJ46" s="48"/>
+      <c r="AK46" s="48"/>
+      <c r="AL46" s="48"/>
+      <c r="AM46" s="48"/>
+      <c r="AN46" s="48"/>
+      <c r="AO46" s="48"/>
+      <c r="AP46" s="48"/>
+      <c r="AQ46" s="48"/>
+      <c r="AR46" s="48"/>
+      <c r="AS46" s="48"/>
+      <c r="AT46" s="48"/>
+      <c r="AU46" s="48"/>
+      <c r="AV46" s="48"/>
+      <c r="AW46" s="48"/>
+      <c r="AX46" s="48"/>
+      <c r="AY46" s="48"/>
+      <c r="AZ46" s="48"/>
+      <c r="BA46" s="48"/>
+      <c r="BB46" s="48"/>
+      <c r="BC46" s="48"/>
+      <c r="BD46" s="48"/>
+      <c r="BE46" s="48"/>
+      <c r="BF46" s="48"/>
+      <c r="BG46" s="48"/>
+      <c r="BH46" s="48"/>
+      <c r="BI46" s="48"/>
+      <c r="BJ46" s="48"/>
+      <c r="BK46" s="48"/>
+      <c r="BL46" s="48"/>
+      <c r="BM46" s="48"/>
+      <c r="BN46" s="48"/>
+      <c r="BO46" s="48"/>
+      <c r="BP46" s="48"/>
+      <c r="BQ46" s="48"/>
+      <c r="BR46" s="48"/>
+      <c r="BS46" s="48"/>
+      <c r="BT46" s="48"/>
+      <c r="BU46" s="48"/>
+      <c r="BV46" s="48"/>
+      <c r="BW46" s="48"/>
+      <c r="BX46" s="48"/>
+      <c r="BY46" s="48"/>
+      <c r="BZ46" s="48"/>
+      <c r="CA46" s="48"/>
+      <c r="CB46" s="48"/>
+      <c r="CC46" s="48"/>
+      <c r="CD46" s="48"/>
+      <c r="CE46" s="48"/>
+      <c r="CF46" s="48"/>
+      <c r="CG46" s="48"/>
+      <c r="CH46" s="48"/>
+      <c r="CI46" s="48"/>
+    </row>
+    <row r="47" spans="1:87" ht="14.4">
+      <c r="A47" s="16">
         <v>1</v>
       </c>
-      <c r="B46" s="19" t="s">
+      <c r="B47" s="19" t="s">
         <v>75</v>
-      </c>
-      <c r="C46" s="49"/>
-      <c r="D46" s="49"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="19"/>
-      <c r="G46" s="19"/>
-      <c r="H46" s="19"/>
-      <c r="I46" s="50"/>
-      <c r="J46" s="51"/>
-      <c r="K46" s="21"/>
-      <c r="L46" s="22"/>
-      <c r="M46" s="23"/>
-      <c r="N46" s="23"/>
-      <c r="O46" s="23"/>
-      <c r="P46" s="23"/>
-      <c r="Q46" s="23"/>
-      <c r="R46" s="24"/>
-      <c r="S46" s="24"/>
-      <c r="T46" s="24"/>
-      <c r="U46" s="24"/>
-      <c r="V46" s="24"/>
-      <c r="W46" s="24"/>
-      <c r="X46" s="24"/>
-      <c r="Y46" s="23"/>
-      <c r="Z46" s="23"/>
-      <c r="AA46" s="23"/>
-      <c r="AB46" s="23"/>
-      <c r="AC46" s="23"/>
-      <c r="AD46" s="23"/>
-      <c r="AE46" s="23"/>
-      <c r="AF46" s="24"/>
-      <c r="AG46" s="24"/>
-      <c r="AH46" s="24"/>
-      <c r="AI46" s="24"/>
-      <c r="AJ46" s="24"/>
-      <c r="AK46" s="24"/>
-      <c r="AL46" s="24"/>
-      <c r="AM46" s="25"/>
-      <c r="AN46" s="25"/>
-      <c r="AO46" s="25"/>
-      <c r="AP46" s="25"/>
-      <c r="AQ46" s="25"/>
-      <c r="AR46" s="25"/>
-      <c r="AS46" s="25"/>
-      <c r="AT46" s="24"/>
-      <c r="AU46" s="24"/>
-      <c r="AV46" s="24"/>
-      <c r="AW46" s="24"/>
-      <c r="AX46" s="24"/>
-      <c r="AY46" s="24"/>
-      <c r="AZ46" s="24"/>
-      <c r="BA46" s="25"/>
-      <c r="BB46" s="25"/>
-      <c r="BC46" s="25"/>
-      <c r="BD46" s="25"/>
-      <c r="BE46" s="25"/>
-      <c r="BF46" s="25"/>
-      <c r="BG46" s="25"/>
-      <c r="BH46" s="24"/>
-      <c r="BI46" s="24"/>
-      <c r="BJ46" s="24"/>
-      <c r="BK46" s="24"/>
-      <c r="BL46" s="24"/>
-      <c r="BM46" s="24"/>
-      <c r="BN46" s="24"/>
-      <c r="BO46" s="23"/>
-      <c r="BP46" s="23"/>
-      <c r="BQ46" s="23"/>
-      <c r="BR46" s="23"/>
-      <c r="BS46" s="23"/>
-      <c r="BT46" s="23"/>
-      <c r="BU46" s="23"/>
-      <c r="BV46" s="24"/>
-      <c r="BW46" s="24"/>
-      <c r="BX46" s="24"/>
-      <c r="BY46" s="24"/>
-      <c r="BZ46" s="24"/>
-      <c r="CA46" s="24"/>
-      <c r="CB46" s="24"/>
-      <c r="CC46" s="25"/>
-      <c r="CD46" s="25"/>
-      <c r="CE46" s="25"/>
-      <c r="CF46" s="25"/>
-      <c r="CG46" s="25"/>
-      <c r="CH46" s="25"/>
-      <c r="CI46" s="25"/>
-    </row>
-    <row r="47" spans="1:87">
-      <c r="A47" s="16">
-        <v>2</v>
-      </c>
-      <c r="B47" s="19" t="s">
-        <v>76</v>
       </c>
       <c r="C47" s="49"/>
       <c r="D47" s="49"/>
@@ -7098,10 +7167,12 @@
       <c r="CH47" s="25"/>
       <c r="CI47" s="25"/>
     </row>
-    <row r="48" spans="1:87">
-      <c r="A48" s="16"/>
+    <row r="48" spans="1:87" ht="14.4">
+      <c r="A48" s="16">
+        <v>2</v>
+      </c>
       <c r="B48" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C48" s="49"/>
       <c r="D48" s="49"/>
@@ -7189,12 +7260,10 @@
       <c r="CH48" s="25"/>
       <c r="CI48" s="25"/>
     </row>
-    <row r="49" spans="1:87">
-      <c r="A49" s="16">
-        <v>3</v>
-      </c>
+    <row r="49" spans="1:87" ht="28.8">
+      <c r="A49" s="16"/>
       <c r="B49" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C49" s="49"/>
       <c r="D49" s="49"/>
@@ -7282,10 +7351,12 @@
       <c r="CH49" s="25"/>
       <c r="CI49" s="25"/>
     </row>
-    <row r="50" spans="1:87">
-      <c r="A50" s="16"/>
+    <row r="50" spans="1:87" ht="14.4">
+      <c r="A50" s="16">
+        <v>3</v>
+      </c>
       <c r="B50" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C50" s="49"/>
       <c r="D50" s="49"/>
@@ -7373,10 +7444,10 @@
       <c r="CH50" s="25"/>
       <c r="CI50" s="25"/>
     </row>
-    <row r="51" spans="1:87">
+    <row r="51" spans="1:87" ht="14.4">
       <c r="A51" s="16"/>
       <c r="B51" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C51" s="49"/>
       <c r="D51" s="49"/>
@@ -7464,10 +7535,10 @@
       <c r="CH51" s="25"/>
       <c r="CI51" s="25"/>
     </row>
-    <row r="52" spans="1:87">
+    <row r="52" spans="1:87" ht="14.4">
       <c r="A52" s="16"/>
       <c r="B52" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C52" s="49"/>
       <c r="D52" s="49"/>
@@ -7555,12 +7626,10 @@
       <c r="CH52" s="25"/>
       <c r="CI52" s="25"/>
     </row>
-    <row r="53" spans="1:87">
-      <c r="A53" s="16" t="s">
-        <v>56</v>
-      </c>
+    <row r="53" spans="1:87" ht="14.4">
+      <c r="A53" s="16"/>
       <c r="B53" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C53" s="49"/>
       <c r="D53" s="49"/>
@@ -7630,7 +7699,7 @@
       <c r="BP53" s="23"/>
       <c r="BQ53" s="23"/>
       <c r="BR53" s="23"/>
-      <c r="BS53" s="52"/>
+      <c r="BS53" s="23"/>
       <c r="BT53" s="23"/>
       <c r="BU53" s="23"/>
       <c r="BV53" s="24"/>
@@ -7648,120 +7717,196 @@
       <c r="CH53" s="25"/>
       <c r="CI53" s="25"/>
     </row>
-    <row r="54" spans="1:87" ht="15.75" customHeight="1">
-      <c r="A54" s="55" t="s">
+    <row r="54" spans="1:87" ht="14.4">
+      <c r="A54" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C54" s="49"/>
+      <c r="D54" s="49"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="19"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="19"/>
+      <c r="I54" s="50"/>
+      <c r="J54" s="51"/>
+      <c r="K54" s="21"/>
+      <c r="L54" s="22"/>
+      <c r="M54" s="23"/>
+      <c r="N54" s="23"/>
+      <c r="O54" s="23"/>
+      <c r="P54" s="23"/>
+      <c r="Q54" s="23"/>
+      <c r="R54" s="24"/>
+      <c r="S54" s="24"/>
+      <c r="T54" s="24"/>
+      <c r="U54" s="24"/>
+      <c r="V54" s="24"/>
+      <c r="W54" s="24"/>
+      <c r="X54" s="24"/>
+      <c r="Y54" s="23"/>
+      <c r="Z54" s="23"/>
+      <c r="AA54" s="23"/>
+      <c r="AB54" s="23"/>
+      <c r="AC54" s="23"/>
+      <c r="AD54" s="23"/>
+      <c r="AE54" s="23"/>
+      <c r="AF54" s="24"/>
+      <c r="AG54" s="24"/>
+      <c r="AH54" s="24"/>
+      <c r="AI54" s="24"/>
+      <c r="AJ54" s="24"/>
+      <c r="AK54" s="24"/>
+      <c r="AL54" s="24"/>
+      <c r="AM54" s="25"/>
+      <c r="AN54" s="25"/>
+      <c r="AO54" s="25"/>
+      <c r="AP54" s="25"/>
+      <c r="AQ54" s="25"/>
+      <c r="AR54" s="25"/>
+      <c r="AS54" s="25"/>
+      <c r="AT54" s="24"/>
+      <c r="AU54" s="24"/>
+      <c r="AV54" s="24"/>
+      <c r="AW54" s="24"/>
+      <c r="AX54" s="24"/>
+      <c r="AY54" s="24"/>
+      <c r="AZ54" s="24"/>
+      <c r="BA54" s="25"/>
+      <c r="BB54" s="25"/>
+      <c r="BC54" s="25"/>
+      <c r="BD54" s="25"/>
+      <c r="BE54" s="25"/>
+      <c r="BF54" s="25"/>
+      <c r="BG54" s="25"/>
+      <c r="BH54" s="24"/>
+      <c r="BI54" s="24"/>
+      <c r="BJ54" s="24"/>
+      <c r="BK54" s="24"/>
+      <c r="BL54" s="24"/>
+      <c r="BM54" s="24"/>
+      <c r="BN54" s="24"/>
+      <c r="BO54" s="23"/>
+      <c r="BP54" s="23"/>
+      <c r="BQ54" s="23"/>
+      <c r="BR54" s="23"/>
+      <c r="BS54" s="52"/>
+      <c r="BT54" s="23"/>
+      <c r="BU54" s="23"/>
+      <c r="BV54" s="24"/>
+      <c r="BW54" s="24"/>
+      <c r="BX54" s="24"/>
+      <c r="BY54" s="24"/>
+      <c r="BZ54" s="24"/>
+      <c r="CA54" s="24"/>
+      <c r="CB54" s="24"/>
+      <c r="CC54" s="25"/>
+      <c r="CD54" s="25"/>
+      <c r="CE54" s="25"/>
+      <c r="CF54" s="25"/>
+      <c r="CG54" s="25"/>
+      <c r="CH54" s="25"/>
+      <c r="CI54" s="25"/>
+    </row>
+    <row r="55" spans="1:87" ht="15.75" customHeight="1">
+      <c r="A55" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="B54" s="56"/>
-      <c r="C54" s="56"/>
-      <c r="D54" s="56"/>
-      <c r="E54" s="56"/>
-      <c r="F54" s="56"/>
-      <c r="G54" s="56"/>
-      <c r="H54" s="56"/>
-      <c r="I54" s="56"/>
-      <c r="J54" s="56"/>
-      <c r="K54" s="57"/>
-      <c r="L54" s="58"/>
-      <c r="M54" s="58"/>
-      <c r="N54" s="58"/>
-      <c r="O54" s="58"/>
-      <c r="P54" s="58"/>
-      <c r="Q54" s="58"/>
-      <c r="R54" s="58"/>
-      <c r="S54" s="58"/>
-      <c r="T54" s="58"/>
-      <c r="U54" s="58"/>
-      <c r="V54" s="58"/>
-      <c r="W54" s="58"/>
-      <c r="X54" s="58"/>
-      <c r="Y54" s="58"/>
-      <c r="Z54" s="58"/>
-      <c r="AA54" s="58"/>
-      <c r="AB54" s="58"/>
-      <c r="AC54" s="58"/>
-      <c r="AD54" s="58"/>
-      <c r="AE54" s="58"/>
-      <c r="AF54" s="58"/>
-      <c r="AG54" s="58"/>
-      <c r="AH54" s="58"/>
-      <c r="AI54" s="58"/>
-      <c r="AJ54" s="58"/>
-      <c r="AK54" s="58"/>
-      <c r="AL54" s="58"/>
-      <c r="AM54" s="58"/>
-      <c r="AN54" s="58"/>
-      <c r="AO54" s="58"/>
-      <c r="AP54" s="58"/>
-      <c r="AQ54" s="58"/>
-      <c r="AR54" s="58"/>
-      <c r="AS54" s="58"/>
-      <c r="AT54" s="58"/>
-      <c r="AU54" s="58"/>
-      <c r="AV54" s="58"/>
-      <c r="AW54" s="58"/>
-      <c r="AX54" s="58"/>
-      <c r="AY54" s="58"/>
-      <c r="AZ54" s="58"/>
-      <c r="BA54" s="58"/>
-      <c r="BB54" s="58"/>
-      <c r="BC54" s="58"/>
-      <c r="BD54" s="58"/>
-      <c r="BE54" s="58"/>
-      <c r="BF54" s="58"/>
-      <c r="BG54" s="58"/>
-      <c r="BH54" s="58"/>
-      <c r="BI54" s="58"/>
-      <c r="BJ54" s="58"/>
-      <c r="BK54" s="58"/>
-      <c r="BL54" s="58"/>
-      <c r="BM54" s="58"/>
-      <c r="BN54" s="58"/>
-      <c r="BO54" s="58"/>
-      <c r="BP54" s="58"/>
-      <c r="BQ54" s="58"/>
-      <c r="BR54" s="58"/>
-      <c r="BS54" s="58"/>
-      <c r="BT54" s="58"/>
-      <c r="BU54" s="58"/>
-      <c r="BV54" s="58"/>
-      <c r="BW54" s="58"/>
-      <c r="BX54" s="58"/>
-      <c r="BY54" s="58"/>
-      <c r="BZ54" s="58"/>
-      <c r="CA54" s="58"/>
-      <c r="CB54" s="58"/>
-      <c r="CC54" s="58"/>
-      <c r="CD54" s="58"/>
-      <c r="CE54" s="58"/>
-      <c r="CF54" s="58"/>
-      <c r="CG54" s="58"/>
-      <c r="CH54" s="58"/>
-      <c r="CI54" s="58"/>
-    </row>
-    <row r="55" spans="1:87" ht="15.75" customHeight="1">
-      <c r="A55" s="16">
+      <c r="B55" s="56"/>
+      <c r="C55" s="56"/>
+      <c r="D55" s="56"/>
+      <c r="E55" s="56"/>
+      <c r="F55" s="56"/>
+      <c r="G55" s="56"/>
+      <c r="H55" s="56"/>
+      <c r="I55" s="56"/>
+      <c r="J55" s="56"/>
+      <c r="K55" s="57"/>
+      <c r="L55" s="58"/>
+      <c r="M55" s="58"/>
+      <c r="N55" s="58"/>
+      <c r="O55" s="58"/>
+      <c r="P55" s="58"/>
+      <c r="Q55" s="58"/>
+      <c r="R55" s="58"/>
+      <c r="S55" s="58"/>
+      <c r="T55" s="58"/>
+      <c r="U55" s="58"/>
+      <c r="V55" s="58"/>
+      <c r="W55" s="58"/>
+      <c r="X55" s="58"/>
+      <c r="Y55" s="58"/>
+      <c r="Z55" s="58"/>
+      <c r="AA55" s="58"/>
+      <c r="AB55" s="58"/>
+      <c r="AC55" s="58"/>
+      <c r="AD55" s="58"/>
+      <c r="AE55" s="58"/>
+      <c r="AF55" s="58"/>
+      <c r="AG55" s="58"/>
+      <c r="AH55" s="58"/>
+      <c r="AI55" s="58"/>
+      <c r="AJ55" s="58"/>
+      <c r="AK55" s="58"/>
+      <c r="AL55" s="58"/>
+      <c r="AM55" s="58"/>
+      <c r="AN55" s="58"/>
+      <c r="AO55" s="58"/>
+      <c r="AP55" s="58"/>
+      <c r="AQ55" s="58"/>
+      <c r="AR55" s="58"/>
+      <c r="AS55" s="58"/>
+      <c r="AT55" s="58"/>
+      <c r="AU55" s="58"/>
+      <c r="AV55" s="58"/>
+      <c r="AW55" s="58"/>
+      <c r="AX55" s="58"/>
+      <c r="AY55" s="58"/>
+      <c r="AZ55" s="58"/>
+      <c r="BA55" s="58"/>
+      <c r="BB55" s="58"/>
+      <c r="BC55" s="58"/>
+      <c r="BD55" s="58"/>
+      <c r="BE55" s="58"/>
+      <c r="BF55" s="58"/>
+      <c r="BG55" s="58"/>
+      <c r="BH55" s="58"/>
+      <c r="BI55" s="58"/>
+      <c r="BJ55" s="58"/>
+      <c r="BK55" s="58"/>
+      <c r="BL55" s="58"/>
+      <c r="BM55" s="58"/>
+      <c r="BN55" s="58"/>
+      <c r="BO55" s="58"/>
+      <c r="BP55" s="58"/>
+      <c r="BQ55" s="58"/>
+      <c r="BR55" s="58"/>
+      <c r="BS55" s="58"/>
+      <c r="BT55" s="58"/>
+      <c r="BU55" s="58"/>
+      <c r="BV55" s="58"/>
+      <c r="BW55" s="58"/>
+      <c r="BX55" s="58"/>
+      <c r="BY55" s="58"/>
+      <c r="BZ55" s="58"/>
+      <c r="CA55" s="58"/>
+      <c r="CB55" s="58"/>
+      <c r="CC55" s="58"/>
+      <c r="CD55" s="58"/>
+      <c r="CE55" s="58"/>
+      <c r="CF55" s="58"/>
+      <c r="CG55" s="58"/>
+      <c r="CH55" s="58"/>
+      <c r="CI55" s="58"/>
+    </row>
+    <row r="56" spans="1:87" ht="15.75" customHeight="1">
+      <c r="A56" s="16">
         <v>1</v>
       </c>
-      <c r="B55" s="16" t="s">
+      <c r="B56" s="16" t="s">
         <v>84</v>
-      </c>
-      <c r="C55" s="59"/>
-      <c r="D55" s="59"/>
-      <c r="E55" s="59"/>
-      <c r="F55" s="59"/>
-      <c r="G55" s="59"/>
-      <c r="H55" s="59"/>
-      <c r="I55" s="59"/>
-      <c r="J55" s="59"/>
-      <c r="K55" s="60"/>
-    </row>
-    <row r="56" spans="1:87" ht="15.75" customHeight="1">
-      <c r="A56" s="61">
-        <v>2</v>
-      </c>
-      <c r="B56" s="16" t="s">
-        <v>85</v>
       </c>
       <c r="C56" s="59"/>
       <c r="D56" s="59"/>
@@ -7774,9 +7919,11 @@
       <c r="K56" s="60"/>
     </row>
     <row r="57" spans="1:87" ht="15.75" customHeight="1">
-      <c r="A57" s="61"/>
+      <c r="A57" s="61">
+        <v>2</v>
+      </c>
       <c r="B57" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C57" s="59"/>
       <c r="D57" s="59"/>
@@ -7791,7 +7938,7 @@
     <row r="58" spans="1:87" ht="15.75" customHeight="1">
       <c r="A58" s="61"/>
       <c r="B58" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C58" s="59"/>
       <c r="D58" s="59"/>
@@ -7806,7 +7953,7 @@
     <row r="59" spans="1:87" ht="15.75" customHeight="1">
       <c r="A59" s="61"/>
       <c r="B59" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C59" s="59"/>
       <c r="D59" s="59"/>
@@ -7819,11 +7966,9 @@
       <c r="K59" s="60"/>
     </row>
     <row r="60" spans="1:87" ht="15.75" customHeight="1">
-      <c r="A60" s="61" t="s">
-        <v>56</v>
-      </c>
+      <c r="A60" s="61"/>
       <c r="B60" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C60" s="59"/>
       <c r="D60" s="59"/>
@@ -7834,11 +7979,24 @@
       <c r="I60" s="59"/>
       <c r="J60" s="59"/>
       <c r="K60" s="60"/>
-      <c r="CG60" s="62"/>
     </row>
     <row r="61" spans="1:87" ht="15.75" customHeight="1">
-      <c r="A61" s="60"/>
+      <c r="A61" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="B61" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C61" s="59"/>
+      <c r="D61" s="59"/>
+      <c r="E61" s="59"/>
+      <c r="F61" s="59"/>
+      <c r="G61" s="59"/>
+      <c r="H61" s="59"/>
+      <c r="I61" s="59"/>
+      <c r="J61" s="59"/>
       <c r="K61" s="60"/>
+      <c r="CG61" s="62"/>
     </row>
     <row r="62" spans="1:87" ht="15.75" customHeight="1">
       <c r="A62" s="60"/>
@@ -11590,87 +11748,87 @@
     </row>
     <row r="999" spans="1:87" ht="15.75" customHeight="1">
       <c r="A999" s="60"/>
-      <c r="K999" s="92"/>
-      <c r="L999" s="65"/>
-      <c r="M999" s="65"/>
-      <c r="N999" s="65"/>
-      <c r="O999" s="65"/>
-      <c r="P999" s="65"/>
-      <c r="Q999" s="65"/>
-      <c r="R999" s="65"/>
-      <c r="S999" s="65"/>
-      <c r="T999" s="65"/>
-      <c r="U999" s="65"/>
-      <c r="V999" s="65"/>
-      <c r="W999" s="65"/>
-      <c r="X999" s="65"/>
-      <c r="Y999" s="65"/>
-      <c r="Z999" s="65"/>
-      <c r="AA999" s="65"/>
-      <c r="AB999" s="65"/>
-      <c r="AC999" s="65"/>
-      <c r="AD999" s="65"/>
-      <c r="AE999" s="65"/>
-      <c r="AF999" s="65"/>
-      <c r="AG999" s="65"/>
-      <c r="AH999" s="65"/>
-      <c r="AI999" s="65"/>
-      <c r="AJ999" s="65"/>
-      <c r="AK999" s="65"/>
-      <c r="AL999" s="65"/>
-      <c r="AM999" s="65"/>
-      <c r="AN999" s="65"/>
-      <c r="AO999" s="65"/>
-      <c r="AP999" s="65"/>
-      <c r="AQ999" s="65"/>
-      <c r="AR999" s="65"/>
-      <c r="AS999" s="65"/>
-      <c r="AT999" s="65"/>
-      <c r="AU999" s="65"/>
-      <c r="AV999" s="65"/>
-      <c r="AW999" s="65"/>
-      <c r="AX999" s="65"/>
-      <c r="AY999" s="65"/>
-      <c r="AZ999" s="65"/>
-      <c r="BA999" s="65"/>
-      <c r="BB999" s="65"/>
-      <c r="BC999" s="65"/>
-      <c r="BD999" s="65"/>
-      <c r="BE999" s="65"/>
-      <c r="BF999" s="65"/>
-      <c r="BG999" s="65"/>
-      <c r="BH999" s="65"/>
-      <c r="BI999" s="65"/>
-      <c r="BJ999" s="65"/>
-      <c r="BK999" s="65"/>
-      <c r="BL999" s="65"/>
-      <c r="BM999" s="65"/>
-      <c r="BN999" s="65"/>
-      <c r="BO999" s="65"/>
-      <c r="BP999" s="65"/>
-      <c r="BQ999" s="65"/>
-      <c r="BR999" s="65"/>
-      <c r="BS999" s="65"/>
-      <c r="BT999" s="65"/>
-      <c r="BU999" s="65"/>
-      <c r="BV999" s="65"/>
-      <c r="BW999" s="65"/>
-      <c r="BX999" s="65"/>
-      <c r="BY999" s="65"/>
-      <c r="BZ999" s="65"/>
-      <c r="CA999" s="65"/>
-      <c r="CB999" s="65"/>
-      <c r="CC999" s="65"/>
-      <c r="CD999" s="65"/>
-      <c r="CE999" s="65"/>
-      <c r="CF999" s="65"/>
-      <c r="CG999" s="65"/>
-      <c r="CH999" s="65"/>
-      <c r="CI999" s="65"/>
+      <c r="K999" s="60"/>
     </row>
     <row r="1000" spans="1:87" ht="15.75" customHeight="1">
       <c r="A1000" s="60"/>
-      <c r="K1000" s="60"/>
+      <c r="K1000" s="92"/>
+      <c r="L1000" s="65"/>
+      <c r="M1000" s="65"/>
+      <c r="N1000" s="65"/>
+      <c r="O1000" s="65"/>
+      <c r="P1000" s="65"/>
+      <c r="Q1000" s="65"/>
+      <c r="R1000" s="65"/>
+      <c r="S1000" s="65"/>
+      <c r="T1000" s="65"/>
+      <c r="U1000" s="65"/>
+      <c r="V1000" s="65"/>
+      <c r="W1000" s="65"/>
+      <c r="X1000" s="65"/>
+      <c r="Y1000" s="65"/>
+      <c r="Z1000" s="65"/>
+      <c r="AA1000" s="65"/>
+      <c r="AB1000" s="65"/>
+      <c r="AC1000" s="65"/>
+      <c r="AD1000" s="65"/>
+      <c r="AE1000" s="65"/>
+      <c r="AF1000" s="65"/>
+      <c r="AG1000" s="65"/>
+      <c r="AH1000" s="65"/>
+      <c r="AI1000" s="65"/>
+      <c r="AJ1000" s="65"/>
+      <c r="AK1000" s="65"/>
+      <c r="AL1000" s="65"/>
+      <c r="AM1000" s="65"/>
+      <c r="AN1000" s="65"/>
+      <c r="AO1000" s="65"/>
+      <c r="AP1000" s="65"/>
+      <c r="AQ1000" s="65"/>
+      <c r="AR1000" s="65"/>
+      <c r="AS1000" s="65"/>
+      <c r="AT1000" s="65"/>
+      <c r="AU1000" s="65"/>
+      <c r="AV1000" s="65"/>
+      <c r="AW1000" s="65"/>
+      <c r="AX1000" s="65"/>
+      <c r="AY1000" s="65"/>
+      <c r="AZ1000" s="65"/>
+      <c r="BA1000" s="65"/>
+      <c r="BB1000" s="65"/>
+      <c r="BC1000" s="65"/>
+      <c r="BD1000" s="65"/>
+      <c r="BE1000" s="65"/>
+      <c r="BF1000" s="65"/>
+      <c r="BG1000" s="65"/>
+      <c r="BH1000" s="65"/>
+      <c r="BI1000" s="65"/>
+      <c r="BJ1000" s="65"/>
+      <c r="BK1000" s="65"/>
+      <c r="BL1000" s="65"/>
+      <c r="BM1000" s="65"/>
+      <c r="BN1000" s="65"/>
+      <c r="BO1000" s="65"/>
+      <c r="BP1000" s="65"/>
+      <c r="BQ1000" s="65"/>
+      <c r="BR1000" s="65"/>
+      <c r="BS1000" s="65"/>
+      <c r="BT1000" s="65"/>
+      <c r="BU1000" s="65"/>
+      <c r="BV1000" s="65"/>
+      <c r="BW1000" s="65"/>
+      <c r="BX1000" s="65"/>
+      <c r="BY1000" s="65"/>
+      <c r="BZ1000" s="65"/>
+      <c r="CA1000" s="65"/>
+      <c r="CB1000" s="65"/>
+      <c r="CC1000" s="65"/>
+      <c r="CD1000" s="65"/>
+      <c r="CE1000" s="65"/>
+      <c r="CF1000" s="65"/>
+      <c r="CG1000" s="65"/>
+      <c r="CH1000" s="65"/>
+      <c r="CI1000" s="65"/>
     </row>
     <row r="1001" spans="1:87" ht="15.75" customHeight="1">
       <c r="A1001" s="60"/>
@@ -11757,27 +11915,23 @@
       <c r="K1021" s="60"/>
     </row>
     <row r="1022" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A1022" s="92"/>
-      <c r="B1022" s="65"/>
-      <c r="C1022" s="65"/>
-      <c r="D1022" s="65"/>
-      <c r="E1022" s="65"/>
-      <c r="F1022" s="65"/>
-      <c r="G1022" s="65"/>
-      <c r="H1022" s="65"/>
-      <c r="I1022" s="65"/>
+      <c r="A1022" s="60"/>
       <c r="K1022" s="60"/>
+    </row>
+    <row r="1023" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A1023" s="92"/>
+      <c r="B1023" s="65"/>
+      <c r="C1023" s="65"/>
+      <c r="D1023" s="65"/>
+      <c r="E1023" s="65"/>
+      <c r="F1023" s="65"/>
+      <c r="G1023" s="65"/>
+      <c r="H1023" s="65"/>
+      <c r="I1023" s="65"/>
+      <c r="K1023" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="C21:I21"/>
-    <mergeCell ref="C45:I45"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="R1:V1"/>
@@ -11793,8 +11947,16 @@
     <mergeCell ref="BH1:BL1"/>
     <mergeCell ref="BO1:BS1"/>
     <mergeCell ref="BV1:BZ1"/>
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="C22:I22"/>
+    <mergeCell ref="C46:I46"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
   </mergeCells>
-  <conditionalFormatting sqref="J4:J20 I5:I20 I22:J28 I30:J44 I46:J53">
+  <conditionalFormatting sqref="J4:J21 I5:I21 I23:J29 I31:J45 I47:J54">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="percent" val="0"/>
@@ -11815,7 +11977,9 @@
   </sheetPr>
   <dimension ref="A1:AJ51"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -11915,14 +12079,14 @@
       <c r="B3" s="64"/>
       <c r="C3" s="64"/>
       <c r="D3" s="64"/>
-      <c r="E3" s="107" t="str">
+      <c r="E3" s="108" t="str">
         <f>HYPERLINK("https://www.teamgantt.com/signup?utm_source=google-sheets-gantt-template&amp;utm_medium=download&amp;utm_campaign=google-sheets-gantt-template","Build better gantt charts with TeamGantt for FREE!")</f>
         <v>Build better gantt charts with TeamGantt for FREE!</v>
       </c>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="108"/>
-      <c r="I3" s="108"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="109"/>
       <c r="J3" s="74"/>
       <c r="K3" s="74"/>
       <c r="L3" s="74"/>
@@ -12023,7 +12187,7 @@
       <c r="AI5" s="59"/>
       <c r="AJ5" s="59"/>
     </row>
-    <row r="6" spans="1:36">
+    <row r="6" spans="1:36" ht="14.4">
       <c r="A6" s="70" t="s">
         <v>91</v>
       </c>
@@ -12063,81 +12227,81 @@
       <c r="AI6" s="72"/>
       <c r="AJ6" s="71"/>
     </row>
-    <row r="7" spans="1:36">
-      <c r="A7" s="97"/>
-      <c r="B7" s="97" t="s">
+    <row r="7" spans="1:36" ht="14.4">
+      <c r="A7" s="99"/>
+      <c r="B7" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="97" t="s">
+      <c r="C7" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="97" t="s">
+      <c r="D7" s="99" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="97" t="s">
+      <c r="E7" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="97" t="s">
+      <c r="F7" s="99" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="97" t="s">
+      <c r="G7" s="99" t="s">
         <v>102</v>
       </c>
-      <c r="H7" s="97" t="s">
+      <c r="H7" s="99" t="s">
         <v>103</v>
       </c>
-      <c r="I7" s="97" t="s">
+      <c r="I7" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="97" t="s">
+      <c r="J7" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="105"/>
-      <c r="L7" s="98"/>
-      <c r="M7" s="98"/>
-      <c r="N7" s="98"/>
-      <c r="O7" s="98"/>
-      <c r="P7" s="105" t="s">
+      <c r="K7" s="111"/>
+      <c r="L7" s="100"/>
+      <c r="M7" s="100"/>
+      <c r="N7" s="100"/>
+      <c r="O7" s="100"/>
+      <c r="P7" s="111" t="s">
         <v>94</v>
       </c>
-      <c r="Q7" s="98"/>
-      <c r="R7" s="98"/>
-      <c r="S7" s="98"/>
-      <c r="T7" s="98"/>
-      <c r="U7" s="106" t="s">
+      <c r="Q7" s="100"/>
+      <c r="R7" s="100"/>
+      <c r="S7" s="100"/>
+      <c r="T7" s="100"/>
+      <c r="U7" s="110" t="s">
         <v>95</v>
       </c>
-      <c r="V7" s="98"/>
-      <c r="W7" s="98"/>
-      <c r="X7" s="98"/>
-      <c r="Y7" s="98"/>
-      <c r="Z7" s="105" t="s">
+      <c r="V7" s="100"/>
+      <c r="W7" s="100"/>
+      <c r="X7" s="100"/>
+      <c r="Y7" s="100"/>
+      <c r="Z7" s="111" t="s">
         <v>96</v>
       </c>
-      <c r="AA7" s="98"/>
-      <c r="AB7" s="98"/>
-      <c r="AC7" s="98"/>
-      <c r="AD7" s="98"/>
-      <c r="AE7" s="106" t="s">
+      <c r="AA7" s="100"/>
+      <c r="AB7" s="100"/>
+      <c r="AC7" s="100"/>
+      <c r="AD7" s="100"/>
+      <c r="AE7" s="110" t="s">
         <v>97</v>
       </c>
-      <c r="AF7" s="98"/>
-      <c r="AG7" s="98"/>
-      <c r="AH7" s="98"/>
-      <c r="AI7" s="98"/>
+      <c r="AF7" s="100"/>
+      <c r="AG7" s="100"/>
+      <c r="AH7" s="100"/>
+      <c r="AI7" s="100"/>
       <c r="AJ7" s="71"/>
     </row>
-    <row r="8" spans="1:36">
-      <c r="A8" s="98"/>
-      <c r="B8" s="98"/>
-      <c r="C8" s="98"/>
-      <c r="D8" s="98"/>
-      <c r="E8" s="98"/>
-      <c r="F8" s="98"/>
-      <c r="G8" s="98"/>
-      <c r="H8" s="98"/>
-      <c r="I8" s="98"/>
-      <c r="J8" s="98"/>
+    <row r="8" spans="1:36" ht="14.4">
+      <c r="A8" s="100"/>
+      <c r="B8" s="100"/>
+      <c r="C8" s="100"/>
+      <c r="D8" s="100"/>
+      <c r="E8" s="100"/>
+      <c r="F8" s="100"/>
+      <c r="G8" s="100"/>
+      <c r="H8" s="100"/>
+      <c r="I8" s="100"/>
+      <c r="J8" s="100"/>
       <c r="K8" s="71"/>
       <c r="L8" s="71"/>
       <c r="M8" s="71"/>
@@ -12165,7 +12329,7 @@
       <c r="AI8" s="71"/>
       <c r="AJ8" s="71"/>
     </row>
-    <row r="9" spans="1:36">
+    <row r="9" spans="1:36" ht="15.6">
       <c r="A9" s="73" t="s">
         <v>98</v>
       </c>
@@ -12205,7 +12369,7 @@
       <c r="AI9" s="75"/>
       <c r="AJ9" s="75"/>
     </row>
-    <row r="10" spans="1:36">
+    <row r="10" spans="1:36" ht="14.4">
       <c r="B10" s="32" t="s">
         <v>99</v>
       </c>
@@ -12264,7 +12428,7 @@
       <c r="AI10" s="59"/>
       <c r="AJ10" s="59"/>
     </row>
-    <row r="11" spans="1:36">
+    <row r="11" spans="1:36" ht="14.4">
       <c r="B11" s="32" t="s">
         <v>105</v>
       </c>
@@ -12323,7 +12487,7 @@
       <c r="AI11" s="59"/>
       <c r="AJ11" s="59"/>
     </row>
-    <row r="12" spans="1:36">
+    <row r="12" spans="1:36" ht="14.4">
       <c r="B12" s="32" t="s">
         <v>107</v>
       </c>
@@ -12382,7 +12546,7 @@
       <c r="AI12" s="59"/>
       <c r="AJ12" s="59"/>
     </row>
-    <row r="13" spans="1:36">
+    <row r="13" spans="1:36" ht="14.4">
       <c r="B13" s="32" t="s">
         <v>109</v>
       </c>
@@ -12415,7 +12579,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="14" spans="1:36">
+    <row r="14" spans="1:36" ht="14.4">
       <c r="B14" s="32" t="s">
         <v>111</v>
       </c>
@@ -12448,7 +12612,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="15" spans="1:36">
+    <row r="15" spans="1:36" ht="15.6">
       <c r="A15" s="73" t="s">
         <v>113</v>
       </c>
@@ -12462,7 +12626,7 @@
       <c r="I15" s="44"/>
       <c r="J15" s="44"/>
     </row>
-    <row r="16" spans="1:36">
+    <row r="16" spans="1:36" ht="14.4">
       <c r="B16" s="32" t="s">
         <v>114</v>
       </c>
@@ -12495,7 +12659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" ht="14.4">
       <c r="B17" s="32" t="s">
         <v>115</v>
       </c>
@@ -12528,7 +12692,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" ht="14.4">
       <c r="B18" s="32" t="s">
         <v>116</v>
       </c>
@@ -12561,7 +12725,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" ht="14.4">
       <c r="B19" s="32" t="s">
         <v>117</v>
       </c>
@@ -12594,7 +12758,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" ht="15.6">
       <c r="A20" s="73" t="s">
         <v>118</v>
       </c>
@@ -12608,7 +12772,7 @@
       <c r="I20" s="44"/>
       <c r="J20" s="44"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" ht="14.4">
       <c r="B21" s="32" t="s">
         <v>119</v>
       </c>
@@ -12641,7 +12805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" ht="14.4">
       <c r="B22" s="32" t="s">
         <v>120</v>
       </c>
@@ -12674,7 +12838,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" ht="14.4">
       <c r="B23" s="32" t="s">
         <v>121</v>
       </c>
@@ -12707,7 +12871,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" ht="14.4">
       <c r="B24" s="32" t="s">
         <v>122</v>
       </c>
@@ -12740,7 +12904,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" ht="14.4">
       <c r="B25" s="32" t="s">
         <v>123</v>
       </c>
@@ -13019,7 +13183,9 @@
   </sheetPr>
   <dimension ref="A1:AH50"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -13107,16 +13273,16 @@
       <c r="AH2" s="59"/>
     </row>
     <row r="3" spans="1:34" ht="15.75" customHeight="1">
-      <c r="A3" s="109" t="s">
+      <c r="A3" s="112" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="108"/>
-      <c r="C3" s="108"/>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="108"/>
+      <c r="B3" s="109"/>
+      <c r="C3" s="109"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
       <c r="I3" s="66"/>
       <c r="J3" s="67"/>
       <c r="K3" s="67"/>
@@ -13180,7 +13346,7 @@
       <c r="AG4" s="59"/>
       <c r="AH4" s="59"/>
     </row>
-    <row r="5" spans="1:34">
+    <row r="5" spans="1:34" ht="13.8">
       <c r="A5" s="70" t="s">
         <v>91</v>
       </c>
@@ -13217,73 +13383,73 @@
       <c r="AG5" s="59"/>
       <c r="AH5" s="59"/>
     </row>
-    <row r="6" spans="1:34">
-      <c r="A6" s="97"/>
-      <c r="B6" s="97" t="s">
+    <row r="6" spans="1:34" ht="14.4">
+      <c r="A6" s="99"/>
+      <c r="B6" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="97" t="s">
+      <c r="C6" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="97" t="s">
+      <c r="D6" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="97" t="s">
+      <c r="E6" s="99" t="s">
         <v>92</v>
       </c>
-      <c r="F6" s="97" t="s">
+      <c r="F6" s="99" t="s">
         <v>93</v>
       </c>
-      <c r="G6" s="97" t="s">
+      <c r="G6" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="97" t="s">
+      <c r="H6" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="105"/>
-      <c r="J6" s="98"/>
-      <c r="K6" s="98"/>
-      <c r="L6" s="98"/>
-      <c r="M6" s="98"/>
-      <c r="N6" s="105" t="s">
+      <c r="I6" s="111"/>
+      <c r="J6" s="100"/>
+      <c r="K6" s="100"/>
+      <c r="L6" s="100"/>
+      <c r="M6" s="100"/>
+      <c r="N6" s="111" t="s">
         <v>94</v>
       </c>
-      <c r="O6" s="98"/>
-      <c r="P6" s="98"/>
-      <c r="Q6" s="98"/>
-      <c r="R6" s="98"/>
-      <c r="S6" s="106" t="s">
+      <c r="O6" s="100"/>
+      <c r="P6" s="100"/>
+      <c r="Q6" s="100"/>
+      <c r="R6" s="100"/>
+      <c r="S6" s="110" t="s">
         <v>95</v>
       </c>
-      <c r="T6" s="98"/>
-      <c r="U6" s="98"/>
-      <c r="V6" s="98"/>
-      <c r="W6" s="98"/>
-      <c r="X6" s="105" t="s">
+      <c r="T6" s="100"/>
+      <c r="U6" s="100"/>
+      <c r="V6" s="100"/>
+      <c r="W6" s="100"/>
+      <c r="X6" s="111" t="s">
         <v>96</v>
       </c>
-      <c r="Y6" s="98"/>
-      <c r="Z6" s="98"/>
-      <c r="AA6" s="98"/>
-      <c r="AB6" s="98"/>
-      <c r="AC6" s="106" t="s">
+      <c r="Y6" s="100"/>
+      <c r="Z6" s="100"/>
+      <c r="AA6" s="100"/>
+      <c r="AB6" s="100"/>
+      <c r="AC6" s="110" t="s">
         <v>97</v>
       </c>
-      <c r="AD6" s="98"/>
-      <c r="AE6" s="98"/>
-      <c r="AF6" s="98"/>
-      <c r="AG6" s="98"/>
+      <c r="AD6" s="100"/>
+      <c r="AE6" s="100"/>
+      <c r="AF6" s="100"/>
+      <c r="AG6" s="100"/>
       <c r="AH6" s="71"/>
     </row>
-    <row r="7" spans="1:34">
-      <c r="A7" s="98"/>
-      <c r="B7" s="98"/>
-      <c r="C7" s="98"/>
-      <c r="D7" s="98"/>
-      <c r="E7" s="98"/>
-      <c r="F7" s="98"/>
-      <c r="G7" s="98"/>
-      <c r="H7" s="98"/>
+    <row r="7" spans="1:34" ht="14.4">
+      <c r="A7" s="100"/>
+      <c r="B7" s="100"/>
+      <c r="C7" s="100"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="100"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="100"/>
       <c r="I7" s="71"/>
       <c r="J7" s="71"/>
       <c r="K7" s="71"/>
@@ -13311,7 +13477,7 @@
       <c r="AG7" s="71"/>
       <c r="AH7" s="71"/>
     </row>
-    <row r="8" spans="1:34">
+    <row r="8" spans="1:34" ht="15.6">
       <c r="A8" s="73" t="s">
         <v>98</v>
       </c>
@@ -13349,7 +13515,7 @@
       <c r="AG8" s="75"/>
       <c r="AH8" s="75"/>
     </row>
-    <row r="9" spans="1:34">
+    <row r="9" spans="1:34" ht="14.4">
       <c r="B9" s="32" t="s">
         <v>99</v>
       </c>
@@ -13400,7 +13566,7 @@
       <c r="AG9" s="59"/>
       <c r="AH9" s="59"/>
     </row>
-    <row r="10" spans="1:34">
+    <row r="10" spans="1:34" ht="14.4">
       <c r="B10" s="32" t="s">
         <v>105</v>
       </c>
@@ -13451,7 +13617,7 @@
       <c r="AG10" s="59"/>
       <c r="AH10" s="59"/>
     </row>
-    <row r="11" spans="1:34">
+    <row r="11" spans="1:34" ht="14.4">
       <c r="B11" s="32" t="s">
         <v>107</v>
       </c>
@@ -13502,7 +13668,7 @@
       <c r="AG11" s="59"/>
       <c r="AH11" s="59"/>
     </row>
-    <row r="12" spans="1:34">
+    <row r="12" spans="1:34" ht="14.4">
       <c r="B12" s="32" t="s">
         <v>109</v>
       </c>
@@ -13527,7 +13693,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="13" spans="1:34">
+    <row r="13" spans="1:34" ht="14.4">
       <c r="B13" s="32" t="s">
         <v>111</v>
       </c>
@@ -13552,7 +13718,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="14" spans="1:34">
+    <row r="14" spans="1:34" ht="15.6">
       <c r="A14" s="73" t="s">
         <v>113</v>
       </c>
@@ -13564,7 +13730,7 @@
       <c r="G14" s="44"/>
       <c r="H14" s="44"/>
     </row>
-    <row r="15" spans="1:34">
+    <row r="15" spans="1:34" ht="14.4">
       <c r="B15" s="32" t="s">
         <v>114</v>
       </c>
@@ -13589,7 +13755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:34">
+    <row r="16" spans="1:34" ht="14.4">
       <c r="B16" s="32" t="s">
         <v>115</v>
       </c>
@@ -13614,7 +13780,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" ht="14.4">
       <c r="B17" s="32" t="s">
         <v>116</v>
       </c>
@@ -13639,7 +13805,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" ht="14.4">
       <c r="B18" s="32" t="s">
         <v>117</v>
       </c>
@@ -13664,7 +13830,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" ht="15.6">
       <c r="A19" s="73" t="s">
         <v>118</v>
       </c>
@@ -13676,7 +13842,7 @@
       <c r="G19" s="44"/>
       <c r="H19" s="44"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" ht="14.4">
       <c r="B20" s="32" t="s">
         <v>119</v>
       </c>
@@ -13701,7 +13867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" ht="14.4">
       <c r="B21" s="32" t="s">
         <v>120</v>
       </c>
@@ -13726,7 +13892,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" ht="14.4">
       <c r="B22" s="32" t="s">
         <v>121</v>
       </c>
@@ -13751,7 +13917,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" ht="14.4">
       <c r="B23" s="32" t="s">
         <v>122</v>
       </c>
@@ -13776,7 +13942,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" ht="14.4">
       <c r="B24" s="32" t="s">
         <v>123</v>
       </c>
@@ -13801,7 +13967,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" ht="15.6">
       <c r="A25" s="73" t="s">
         <v>124</v>
       </c>

</xml_diff>